<commit_message>
Added new DIO PV (changed Epics buffer sizes!). Updated opi and documentation.
</commit_message>
<xml_diff>
--- a/doc/truth_table_safety_plc.xlsx
+++ b/doc/truth_table_safety_plc.xlsx
@@ -10,16 +10,17 @@
     <sheet name="TRUE TABLE" sheetId="7" r:id="rId1"/>
     <sheet name="EE" sheetId="9" r:id="rId2"/>
     <sheet name="PC" sheetId="10" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'TRUE TABLE'!$A$1:$Q$78</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'TRUE TABLE'!$A$1:$Q$79</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="341">
   <si>
     <t>NA</t>
   </si>
@@ -1208,30 +1209,6 @@
     <t>GERSEMI_V_LEAD_4</t>
   </si>
   <si>
-    <t>GERSEMI_LEAD_1_TEMP</t>
-  </si>
-  <si>
-    <t>GERSEMI_LEAD_2_TEMP</t>
-  </si>
-  <si>
-    <t>GERSEMI_LEAD_3_TEMP</t>
-  </si>
-  <si>
-    <t>GERSEMI_LEAD_4_TEMP</t>
-  </si>
-  <si>
-    <t>Thermoswitch on lead 1 (PC_1)</t>
-  </si>
-  <si>
-    <t>Thermoswitch on lead 2 (PC_1)</t>
-  </si>
-  <si>
-    <t>Thermoswitch on lead 3 (PC_2)</t>
-  </si>
-  <si>
-    <t>Thermoswitch on lead 4 (PC_2)</t>
-  </si>
-  <si>
     <t>Gersemi parameter</t>
   </si>
   <si>
@@ -1341,18 +1318,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ethernet </t>
-  </si>
-  <si>
-    <t>Over the network from Gersemi PLC. There is no thermo-switch. The signal can be generated based on ET650</t>
-  </si>
-  <si>
-    <t>Over the network from Gersemi PLC. There is no thermo-switch. The signal can be generated based on ET651</t>
-  </si>
-  <si>
-    <t>Over the network from Gersemi PLC. There is no thermo-switch. The signal can be generated based on ET652</t>
-  </si>
-  <si>
-    <t>Over the network from Gersemi PLC. There is no thermo-switch. The signal can be generated based on ET653</t>
   </si>
   <si>
     <t>Q1.1</t>
@@ -1396,9 +1361,6 @@
     </r>
   </si>
   <si>
-    <t>EPICS core name</t>
-  </si>
-  <si>
     <t>Q0.1</t>
   </si>
   <si>
@@ -1409,6 +1371,195 @@
   </si>
   <si>
     <t>Q2.2</t>
+  </si>
+  <si>
+    <t>$(P):QuenchStat</t>
+  </si>
+  <si>
+    <t>EPICS core name P=CstatV-MagLPS</t>
+  </si>
+  <si>
+    <t>$(P):DAQ_OK</t>
+  </si>
+  <si>
+    <t>$(P):EE-1:PwrPerm</t>
+  </si>
+  <si>
+    <t>$(P):EE-1:Remote</t>
+  </si>
+  <si>
+    <t>$(P):EE-1:NoError</t>
+  </si>
+  <si>
+    <t>$(P):EE-1:Closed</t>
+  </si>
+  <si>
+    <t>$(P):EE-1:Warn</t>
+  </si>
+  <si>
+    <t>$(P):EE-1:SPAstat</t>
+  </si>
+  <si>
+    <t>$(P):EE-2:PwrPerm</t>
+  </si>
+  <si>
+    <t>$(P):EE-2:Remote</t>
+  </si>
+  <si>
+    <t>$(P):EE-2:NoError</t>
+  </si>
+  <si>
+    <t>$(P):EE-2:Closed</t>
+  </si>
+  <si>
+    <t>$(P):EE-2:Warn</t>
+  </si>
+  <si>
+    <t>$(P):EE-2:SPAstat</t>
+  </si>
+  <si>
+    <t>$(P):PC-1:PwrFail</t>
+  </si>
+  <si>
+    <t>$(P):PC-1:Connected</t>
+  </si>
+  <si>
+    <t>$(P):PC-1:sOn</t>
+  </si>
+  <si>
+    <t>$(P):PC-2:PwrFail</t>
+  </si>
+  <si>
+    <t>$(P):PC-2:Connected</t>
+  </si>
+  <si>
+    <t>$(P):PC-2:sOn</t>
+  </si>
+  <si>
+    <t>$(P):DC24V:PLC</t>
+  </si>
+  <si>
+    <t>$(P):DC24V:Aux</t>
+  </si>
+  <si>
+    <t>$(P):EmgcyBtn</t>
+  </si>
+  <si>
+    <t>$(P):Cbl:Pos</t>
+  </si>
+  <si>
+    <t>$(P):CRYO_1_9K</t>
+  </si>
+  <si>
+    <t>$(P):CRYO_4_5_K</t>
+  </si>
+  <si>
+    <t>$(P):CRYO_LEADS_OK</t>
+  </si>
+  <si>
+    <t>$(P):LEAD1:T_OK</t>
+  </si>
+  <si>
+    <t>$(P):LEAD2:T_OK</t>
+  </si>
+  <si>
+    <t>$(P):LEAD3:T_OK</t>
+  </si>
+  <si>
+    <t>$(P):LEAD4:T_OK</t>
+  </si>
+  <si>
+    <t>$(P):PC:DirectPA</t>
+  </si>
+  <si>
+    <t>$(P):EE-1:CloseCmd</t>
+  </si>
+  <si>
+    <t>$(P):EE-1:RstCmd</t>
+  </si>
+  <si>
+    <t>$(P):EE-2:CloseCmd</t>
+  </si>
+  <si>
+    <t>$(P):EE-2:RstCmd</t>
+  </si>
+  <si>
+    <t>$(P):PC-1:PERM</t>
+  </si>
+  <si>
+    <t>$(P):PC-2:PERM</t>
+  </si>
+  <si>
+    <t>GERSEMI_LEAD_1_VOLT_OK</t>
+  </si>
+  <si>
+    <t>GERSEMI_LEAD_2_VOLT_OK</t>
+  </si>
+  <si>
+    <t>GERSEMI_LEAD_3_VOLT_OK</t>
+  </si>
+  <si>
+    <t>GERSEMI_LEAD_4_VOLT_OK</t>
+  </si>
+  <si>
+    <t>$(P):LEAD1:V_OK</t>
+  </si>
+  <si>
+    <t>$(P):LEAD2:V_OK</t>
+  </si>
+  <si>
+    <t>$(P):LEAD3:V_OK</t>
+  </si>
+  <si>
+    <t>$(P):LEAD4:V_OK</t>
+  </si>
+  <si>
+    <t>Temp. of lead 1 below threshold (PC_1)</t>
+  </si>
+  <si>
+    <t>Temp. of lead 4 below threshold (PC_2)</t>
+  </si>
+  <si>
+    <t>Temp. of lead 3 below threshold (PC_2)</t>
+  </si>
+  <si>
+    <t>Temp. of lead 2 below threshold (PC_1)</t>
+  </si>
+  <si>
+    <t>Voltage drop on lead 1 below threshold (PC_1)</t>
+  </si>
+  <si>
+    <t>Voltage drop on lead 2 below threshold (PC_1)</t>
+  </si>
+  <si>
+    <t>Voltage drop on lead 3 below threshold (PC_2)</t>
+  </si>
+  <si>
+    <t>Voltage drop on lead 4 below threshold (PC_2)</t>
+  </si>
+  <si>
+    <t>Needed only in Gersemi PLC. There is no thermo-switch. The signal can be generated based on ET650</t>
+  </si>
+  <si>
+    <t>Needed only in Gersemi PLC. There is no thermo-switch. The signal can be generated based on ET651</t>
+  </si>
+  <si>
+    <t>Needed only in Gersemi PLC. There is no thermo-switch. The signal can be generated based on ET652</t>
+  </si>
+  <si>
+    <t>Needed only in Gersemi PLC. There is no thermo-switch. The signal can be generated based on ET653</t>
+  </si>
+  <si>
+    <t>Over the network from Gersemi PLC. The signal can be generated based on ET650</t>
+  </si>
+  <si>
+    <t>Over the network from Gersemi PLC. The signal can be generated based on ET651</t>
+  </si>
+  <si>
+    <t>Over the network from Gersemi PLC. The signal can be generated based on ET652</t>
+  </si>
+  <si>
+    <t>Over the network from Gersemi PLC. The signal can be generated based on ET653</t>
   </si>
 </sst>
 </file>
@@ -1570,7 +1721,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="63">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -2306,15 +2457,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -2363,7 +2505,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="281">
+  <cellXfs count="278">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2970,35 +3112,70 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="46" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="13" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -3009,35 +3186,126 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3071,193 +3339,58 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="18" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="42" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="46" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="13" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="18" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="42" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3651,10 +3784,13 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V82"/>
+  <dimension ref="A1:V87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="25" workbookViewId="0">
-      <selection activeCell="L59" sqref="L59"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="25" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3683,7 +3819,7 @@
       <c r="D1" s="180"/>
       <c r="E1" s="180"/>
       <c r="F1" s="181">
-        <v>43770</v>
+        <v>43775</v>
       </c>
       <c r="G1" s="179"/>
       <c r="H1" s="179"/>
@@ -3697,67 +3833,67 @@
       <c r="N1" s="185"/>
     </row>
     <row r="2" spans="1:22" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="224" t="s">
+      <c r="A2" s="243" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="227"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="216" t="s">
+      <c r="B2" s="246"/>
+      <c r="C2" s="247"/>
+      <c r="D2" s="253" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="273" t="s">
-        <v>286</v>
-      </c>
-      <c r="F2" s="216" t="s">
+      <c r="E2" s="261" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="253" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="222" t="s">
+      <c r="G2" s="259" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="223"/>
-      <c r="I2" s="220" t="s">
+      <c r="H2" s="260"/>
+      <c r="I2" s="257" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="220"/>
-      <c r="K2" s="216" t="s">
+      <c r="J2" s="257"/>
+      <c r="K2" s="253" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="218" t="s">
+      <c r="L2" s="255" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="237" t="s">
+      <c r="M2" s="231" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="238"/>
+      <c r="N2" s="232"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="225"/>
-      <c r="B3" s="229"/>
-      <c r="C3" s="230"/>
-      <c r="D3" s="217"/>
-      <c r="E3" s="274"/>
-      <c r="F3" s="217"/>
+      <c r="A3" s="244"/>
+      <c r="B3" s="248"/>
+      <c r="C3" s="249"/>
+      <c r="D3" s="254"/>
+      <c r="E3" s="262"/>
+      <c r="F3" s="254"/>
       <c r="G3" s="88" t="s">
         <v>31</v>
       </c>
       <c r="H3" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="221"/>
-      <c r="J3" s="221"/>
-      <c r="K3" s="221"/>
-      <c r="L3" s="219"/>
-      <c r="M3" s="239"/>
-      <c r="N3" s="240"/>
+      <c r="I3" s="258"/>
+      <c r="J3" s="258"/>
+      <c r="K3" s="258"/>
+      <c r="L3" s="256"/>
+      <c r="M3" s="233"/>
+      <c r="N3" s="234"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:22" s="10" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="226"/>
+      <c r="A4" s="245"/>
       <c r="B4" s="188" t="s">
         <v>16</v>
       </c>
@@ -3774,28 +3910,28 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="190" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="241" t="s">
+      <c r="M4" s="235" t="s">
         <v>106</v>
       </c>
-      <c r="N4" s="242"/>
+      <c r="N4" s="236"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="203" t="s">
+      <c r="A5" s="214" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="231" t="s">
+      <c r="B5" s="250" t="s">
         <v>93</v>
       </c>
       <c r="C5" s="11">
@@ -3820,17 +3956,17 @@
       <c r="L5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="249" t="s">
-        <v>242</v>
-      </c>
-      <c r="N5" s="250"/>
+      <c r="M5" s="241" t="s">
+        <v>234</v>
+      </c>
+      <c r="N5" s="242"/>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
       <c r="Q5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="204"/>
-      <c r="B6" s="232"/>
+      <c r="A6" s="215"/>
+      <c r="B6" s="251"/>
       <c r="C6" s="18">
         <v>2</v>
       </c>
@@ -3853,17 +3989,17 @@
       <c r="L6" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="247" t="s">
-        <v>242</v>
-      </c>
-      <c r="N6" s="248"/>
+      <c r="M6" s="225" t="s">
+        <v>234</v>
+      </c>
+      <c r="N6" s="226"/>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
       <c r="Q6" s="17"/>
     </row>
     <row r="7" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="204"/>
-      <c r="B7" s="232"/>
+      <c r="A7" s="215"/>
+      <c r="B7" s="251"/>
       <c r="C7" s="18">
         <v>3</v>
       </c>
@@ -3877,7 +4013,7 @@
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="22" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="J7" s="24" t="s">
         <v>34</v>
@@ -3886,17 +4022,17 @@
       <c r="L7" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="247" t="s">
-        <v>272</v>
-      </c>
-      <c r="N7" s="248"/>
+      <c r="M7" s="225" t="s">
+        <v>333</v>
+      </c>
+      <c r="N7" s="226"/>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="17"/>
     </row>
     <row r="8" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="204"/>
-      <c r="B8" s="232"/>
+      <c r="A8" s="215"/>
+      <c r="B8" s="251"/>
       <c r="C8" s="18">
         <v>4</v>
       </c>
@@ -3910,7 +4046,7 @@
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="22" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J8" s="24" t="s">
         <v>34</v>
@@ -3919,17 +4055,17 @@
       <c r="L8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="247" t="s">
-        <v>273</v>
-      </c>
-      <c r="N8" s="248"/>
+      <c r="M8" s="225" t="s">
+        <v>334</v>
+      </c>
+      <c r="N8" s="226"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="17"/>
     </row>
     <row r="9" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="204"/>
-      <c r="B9" s="232"/>
+      <c r="A9" s="215"/>
+      <c r="B9" s="251"/>
       <c r="C9" s="18">
         <v>5</v>
       </c>
@@ -3943,7 +4079,7 @@
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="22" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>34</v>
@@ -3952,17 +4088,17 @@
       <c r="L9" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="247" t="s">
-        <v>274</v>
-      </c>
-      <c r="N9" s="248"/>
+      <c r="M9" s="225" t="s">
+        <v>335</v>
+      </c>
+      <c r="N9" s="226"/>
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="17"/>
     </row>
     <row r="10" spans="1:22" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="204"/>
-      <c r="B10" s="233"/>
+      <c r="A10" s="215"/>
+      <c r="B10" s="252"/>
       <c r="C10" s="26">
         <v>6</v>
       </c>
@@ -3976,7 +4112,7 @@
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
       <c r="I10" s="22" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J10" s="30" t="s">
         <v>34</v>
@@ -3985,17 +4121,17 @@
       <c r="L10" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="247" t="s">
-        <v>275</v>
-      </c>
-      <c r="N10" s="248"/>
+      <c r="M10" s="225" t="s">
+        <v>336</v>
+      </c>
+      <c r="N10" s="226"/>
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
     </row>
-    <row r="11" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="204"/>
-      <c r="B11" s="234" t="s">
+    <row r="11" spans="1:22" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="215"/>
+      <c r="B11" s="211" t="s">
         <v>61</v>
       </c>
       <c r="C11" s="33">
@@ -4004,13 +4140,15 @@
       <c r="D11" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="34"/>
+      <c r="E11" s="34" t="s">
+        <v>278</v>
+      </c>
       <c r="F11" s="35" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="36"/>
       <c r="H11" s="36" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="I11" s="37" t="s">
         <v>4</v>
@@ -4024,30 +4162,32 @@
       <c r="L11" s="38">
         <v>1</v>
       </c>
-      <c r="M11" s="243" t="s">
+      <c r="M11" s="237" t="s">
         <v>107</v>
       </c>
-      <c r="N11" s="244"/>
+      <c r="N11" s="238"/>
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="204"/>
-      <c r="B12" s="235"/>
+      <c r="A12" s="215"/>
+      <c r="B12" s="212"/>
       <c r="C12" s="39">
         <v>2</v>
       </c>
       <c r="D12" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="40"/>
+      <c r="E12" s="34" t="s">
+        <v>280</v>
+      </c>
       <c r="F12" s="41" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="42"/>
       <c r="H12" s="42" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="I12" s="43" t="s">
         <v>4</v>
@@ -4061,28 +4201,30 @@
       <c r="L12" s="44">
         <v>1</v>
       </c>
-      <c r="M12" s="245"/>
-      <c r="N12" s="246"/>
+      <c r="M12" s="239"/>
+      <c r="N12" s="240"/>
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="17"/>
     </row>
     <row r="13" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="204"/>
-      <c r="B13" s="235"/>
+      <c r="A13" s="215"/>
+      <c r="B13" s="212"/>
       <c r="C13" s="45">
         <v>3</v>
       </c>
       <c r="D13" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="40"/>
+      <c r="E13" s="40" t="s">
+        <v>281</v>
+      </c>
       <c r="F13" s="41" t="s">
         <v>57</v>
       </c>
       <c r="G13" s="42"/>
       <c r="H13" s="42" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="I13" s="43" t="s">
         <v>4</v>
@@ -4107,21 +4249,23 @@
       <c r="Q13" s="17"/>
     </row>
     <row r="14" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="204"/>
-      <c r="B14" s="235"/>
+      <c r="A14" s="215"/>
+      <c r="B14" s="212"/>
       <c r="C14" s="39">
         <v>4</v>
       </c>
       <c r="D14" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="40"/>
+      <c r="E14" s="40" t="s">
+        <v>282</v>
+      </c>
       <c r="F14" s="41" t="s">
         <v>165</v>
       </c>
       <c r="G14" s="42"/>
       <c r="H14" s="42" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="I14" s="43" t="s">
         <v>4</v>
@@ -4151,21 +4295,23 @@
       <c r="V14" s="49"/>
     </row>
     <row r="15" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="204"/>
-      <c r="B15" s="235"/>
+      <c r="A15" s="215"/>
+      <c r="B15" s="212"/>
       <c r="C15" s="45">
         <v>5</v>
       </c>
       <c r="D15" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="40" t="s">
+        <v>283</v>
+      </c>
       <c r="F15" s="41" t="s">
         <v>24</v>
       </c>
       <c r="G15" s="42"/>
       <c r="H15" s="42" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="I15" s="43" t="s">
         <v>4</v>
@@ -4195,21 +4341,23 @@
       <c r="V15" s="49"/>
     </row>
     <row r="16" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="204"/>
-      <c r="B16" s="235"/>
+      <c r="A16" s="215"/>
+      <c r="B16" s="212"/>
       <c r="C16" s="39">
         <v>6</v>
       </c>
       <c r="D16" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="40"/>
+      <c r="E16" s="40" t="s">
+        <v>284</v>
+      </c>
       <c r="F16" s="41" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="42"/>
       <c r="H16" s="42" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="I16" s="43" t="s">
         <v>4</v>
@@ -4237,21 +4385,23 @@
       <c r="V16" s="49"/>
     </row>
     <row r="17" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="204"/>
-      <c r="B17" s="235"/>
+      <c r="A17" s="215"/>
+      <c r="B17" s="212"/>
       <c r="C17" s="45">
         <v>7</v>
       </c>
       <c r="D17" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="40" t="s">
+        <v>285</v>
+      </c>
       <c r="F17" s="41" t="s">
         <v>174</v>
       </c>
       <c r="G17" s="42"/>
       <c r="H17" s="42" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="I17" s="43" t="s">
         <v>4</v>
@@ -4281,21 +4431,23 @@
       <c r="V17" s="49"/>
     </row>
     <row r="18" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="204"/>
-      <c r="B18" s="235"/>
+      <c r="A18" s="215"/>
+      <c r="B18" s="212"/>
       <c r="C18" s="39">
         <v>8</v>
       </c>
       <c r="D18" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="40"/>
+      <c r="E18" s="40" t="s">
+        <v>286</v>
+      </c>
       <c r="F18" s="50" t="s">
         <v>26</v>
       </c>
       <c r="G18" s="42"/>
       <c r="H18" s="42" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="I18" s="43" t="s">
         <v>4</v>
@@ -4325,21 +4477,23 @@
       <c r="V18" s="49"/>
     </row>
     <row r="19" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="204"/>
-      <c r="B19" s="235"/>
+      <c r="A19" s="215"/>
+      <c r="B19" s="212"/>
       <c r="C19" s="45">
         <v>9</v>
       </c>
       <c r="D19" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="40"/>
+      <c r="E19" s="40" t="s">
+        <v>287</v>
+      </c>
       <c r="F19" s="41" t="s">
         <v>57</v>
       </c>
       <c r="G19" s="42"/>
       <c r="H19" s="42" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="I19" s="43" t="s">
         <v>4</v>
@@ -4369,21 +4523,23 @@
       <c r="V19" s="49"/>
     </row>
     <row r="20" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="204"/>
-      <c r="B20" s="235"/>
+      <c r="A20" s="215"/>
+      <c r="B20" s="212"/>
       <c r="C20" s="39">
         <v>10</v>
       </c>
       <c r="D20" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="40"/>
+      <c r="E20" s="40" t="s">
+        <v>288</v>
+      </c>
       <c r="F20" s="41" t="s">
         <v>165</v>
       </c>
       <c r="G20" s="42"/>
       <c r="H20" s="42" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="I20" s="43" t="s">
         <v>4</v>
@@ -4408,21 +4564,23 @@
       <c r="Q20" s="17"/>
     </row>
     <row r="21" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="204"/>
-      <c r="B21" s="235"/>
+      <c r="A21" s="215"/>
+      <c r="B21" s="212"/>
       <c r="C21" s="45">
         <v>11</v>
       </c>
       <c r="D21" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="40"/>
+      <c r="E21" s="40" t="s">
+        <v>289</v>
+      </c>
       <c r="F21" s="41" t="s">
         <v>24</v>
       </c>
       <c r="G21" s="42"/>
       <c r="H21" s="42" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="I21" s="43" t="s">
         <v>4</v>
@@ -4447,21 +4605,23 @@
       <c r="Q21" s="17"/>
     </row>
     <row r="22" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="204"/>
-      <c r="B22" s="235"/>
+      <c r="A22" s="215"/>
+      <c r="B22" s="212"/>
       <c r="C22" s="39">
         <v>12</v>
       </c>
       <c r="D22" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="40"/>
+      <c r="E22" s="40" t="s">
+        <v>290</v>
+      </c>
       <c r="F22" s="41" t="s">
         <v>25</v>
       </c>
       <c r="G22" s="42"/>
       <c r="H22" s="42" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I22" s="43" t="s">
         <v>4</v>
@@ -4484,21 +4644,23 @@
       <c r="Q22" s="17"/>
     </row>
     <row r="23" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="204"/>
-      <c r="B23" s="235"/>
+      <c r="A23" s="215"/>
+      <c r="B23" s="212"/>
       <c r="C23" s="45">
         <v>13</v>
       </c>
       <c r="D23" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="E23" s="40"/>
+      <c r="E23" s="40" t="s">
+        <v>291</v>
+      </c>
       <c r="F23" s="41" t="s">
         <v>174</v>
       </c>
       <c r="G23" s="42"/>
       <c r="H23" s="42" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="I23" s="43" t="s">
         <v>4</v>
@@ -4523,21 +4685,23 @@
       <c r="Q23" s="17"/>
     </row>
     <row r="24" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="204"/>
-      <c r="B24" s="235"/>
+      <c r="A24" s="215"/>
+      <c r="B24" s="212"/>
       <c r="C24" s="39">
         <v>14</v>
       </c>
       <c r="D24" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="40"/>
+      <c r="E24" s="40" t="s">
+        <v>292</v>
+      </c>
       <c r="F24" s="50" t="s">
         <v>26</v>
       </c>
       <c r="G24" s="42"/>
       <c r="H24" s="42" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="I24" s="43" t="s">
         <v>4</v>
@@ -4562,21 +4726,23 @@
       <c r="Q24" s="17"/>
     </row>
     <row r="25" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="204"/>
-      <c r="B25" s="235"/>
+      <c r="A25" s="215"/>
+      <c r="B25" s="212"/>
       <c r="C25" s="45">
         <v>15</v>
       </c>
       <c r="D25" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="40"/>
+      <c r="E25" s="40" t="s">
+        <v>293</v>
+      </c>
       <c r="F25" s="41" t="s">
         <v>43</v>
       </c>
       <c r="G25" s="42"/>
       <c r="H25" s="42" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="I25" s="43" t="s">
         <v>4</v>
@@ -4590,30 +4756,32 @@
       <c r="L25" s="44">
         <v>1</v>
       </c>
-      <c r="M25" s="253" t="s">
+      <c r="M25" s="223" t="s">
         <v>202</v>
       </c>
-      <c r="N25" s="254"/>
+      <c r="N25" s="224"/>
       <c r="O25" s="17"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="17"/>
     </row>
     <row r="26" spans="1:22" s="53" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="204"/>
-      <c r="B26" s="235"/>
+      <c r="A26" s="215"/>
+      <c r="B26" s="212"/>
       <c r="C26" s="45">
         <v>16</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="40"/>
+      <c r="E26" s="40" t="s">
+        <v>294</v>
+      </c>
       <c r="F26" s="41" t="s">
         <v>46</v>
       </c>
       <c r="G26" s="42"/>
       <c r="H26" s="42" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I26" s="43" t="s">
         <v>4</v>
@@ -4627,30 +4795,32 @@
       <c r="L26" s="44">
         <v>1</v>
       </c>
-      <c r="M26" s="253" t="s">
+      <c r="M26" s="223" t="s">
         <v>50</v>
       </c>
-      <c r="N26" s="254"/>
+      <c r="N26" s="224"/>
       <c r="O26" s="52"/>
       <c r="P26" s="52"/>
       <c r="Q26" s="52"/>
     </row>
     <row r="27" spans="1:22" s="55" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="204"/>
-      <c r="B27" s="235"/>
+      <c r="A27" s="215"/>
+      <c r="B27" s="212"/>
       <c r="C27" s="39">
         <v>17</v>
       </c>
       <c r="D27" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="40"/>
+      <c r="E27" s="40" t="s">
+        <v>295</v>
+      </c>
       <c r="F27" s="41" t="s">
         <v>47</v>
       </c>
       <c r="G27" s="42"/>
       <c r="H27" s="42" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="I27" s="43" t="s">
         <v>4</v>
@@ -4664,30 +4834,32 @@
       <c r="L27" s="44">
         <v>1</v>
       </c>
-      <c r="M27" s="253" t="s">
+      <c r="M27" s="223" t="s">
         <v>218</v>
       </c>
-      <c r="N27" s="254"/>
+      <c r="N27" s="224"/>
       <c r="O27" s="54"/>
       <c r="P27" s="54"/>
       <c r="Q27" s="54"/>
     </row>
     <row r="28" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="204"/>
-      <c r="B28" s="235"/>
+      <c r="A28" s="215"/>
+      <c r="B28" s="212"/>
       <c r="C28" s="45">
         <v>18</v>
       </c>
       <c r="D28" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="40"/>
+      <c r="E28" s="40" t="s">
+        <v>296</v>
+      </c>
       <c r="F28" s="41" t="s">
         <v>43</v>
       </c>
       <c r="G28" s="42"/>
       <c r="H28" s="42" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="I28" s="43" t="s">
         <v>4</v>
@@ -4701,30 +4873,32 @@
       <c r="L28" s="44">
         <v>1</v>
       </c>
-      <c r="M28" s="253" t="s">
+      <c r="M28" s="223" t="s">
         <v>202</v>
       </c>
-      <c r="N28" s="254"/>
+      <c r="N28" s="224"/>
       <c r="O28" s="17"/>
       <c r="P28" s="17"/>
       <c r="Q28" s="17"/>
     </row>
     <row r="29" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="204"/>
-      <c r="B29" s="235"/>
+      <c r="A29" s="215"/>
+      <c r="B29" s="212"/>
       <c r="C29" s="45">
         <v>19</v>
       </c>
       <c r="D29" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="40"/>
+      <c r="E29" s="40" t="s">
+        <v>297</v>
+      </c>
       <c r="F29" s="41" t="s">
         <v>46</v>
       </c>
       <c r="G29" s="42"/>
       <c r="H29" s="42" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="I29" s="43" t="s">
         <v>4</v>
@@ -4738,30 +4912,32 @@
       <c r="L29" s="44">
         <v>1</v>
       </c>
-      <c r="M29" s="253" t="s">
+      <c r="M29" s="223" t="s">
         <v>50</v>
       </c>
-      <c r="N29" s="254"/>
+      <c r="N29" s="224"/>
       <c r="O29" s="17"/>
       <c r="P29" s="17"/>
       <c r="Q29" s="17"/>
     </row>
     <row r="30" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="204"/>
-      <c r="B30" s="235"/>
+      <c r="A30" s="215"/>
+      <c r="B30" s="212"/>
       <c r="C30" s="39">
         <v>20</v>
       </c>
       <c r="D30" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="40"/>
+      <c r="E30" s="40" t="s">
+        <v>298</v>
+      </c>
       <c r="F30" s="41" t="s">
         <v>47</v>
       </c>
       <c r="G30" s="42"/>
       <c r="H30" s="42" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="I30" s="43" t="s">
         <v>4</v>
@@ -4775,30 +4951,32 @@
       <c r="L30" s="44">
         <v>1</v>
       </c>
-      <c r="M30" s="253" t="s">
+      <c r="M30" s="223" t="s">
         <v>218</v>
       </c>
-      <c r="N30" s="254"/>
+      <c r="N30" s="224"/>
       <c r="O30" s="17"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="17"/>
     </row>
     <row r="31" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="204"/>
-      <c r="B31" s="235"/>
+      <c r="A31" s="215"/>
+      <c r="B31" s="212"/>
       <c r="C31" s="45">
         <v>21</v>
       </c>
       <c r="D31" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="40"/>
+      <c r="E31" s="40" t="s">
+        <v>299</v>
+      </c>
       <c r="F31" s="50" t="s">
         <v>67</v>
       </c>
       <c r="G31" s="43"/>
       <c r="H31" s="43" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="I31" s="43" t="s">
         <v>4</v>
@@ -4817,21 +4995,23 @@
       <c r="Q31" s="17"/>
     </row>
     <row r="32" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="204"/>
-      <c r="B32" s="235"/>
+      <c r="A32" s="215"/>
+      <c r="B32" s="212"/>
       <c r="C32" s="45">
         <v>22</v>
       </c>
       <c r="D32" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="40"/>
+      <c r="E32" s="40" t="s">
+        <v>300</v>
+      </c>
       <c r="F32" s="41" t="s">
         <v>66</v>
       </c>
       <c r="G32" s="43"/>
       <c r="H32" s="43" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="I32" s="43" t="s">
         <v>4</v>
@@ -4852,21 +5032,23 @@
       <c r="Q32" s="17"/>
     </row>
     <row r="33" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="204"/>
-      <c r="B33" s="235"/>
+      <c r="A33" s="215"/>
+      <c r="B33" s="212"/>
       <c r="C33" s="45">
         <v>23</v>
       </c>
       <c r="D33" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="40"/>
+      <c r="E33" s="40" t="s">
+        <v>301</v>
+      </c>
       <c r="F33" s="41" t="s">
         <v>177</v>
       </c>
       <c r="G33" s="43"/>
       <c r="H33" s="43" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="I33" s="43" t="s">
         <v>4</v>
@@ -4889,21 +5071,23 @@
       <c r="Q33" s="17"/>
     </row>
     <row r="34" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="204"/>
-      <c r="B34" s="235"/>
+      <c r="A34" s="215"/>
+      <c r="B34" s="212"/>
       <c r="C34" s="45">
         <v>24</v>
       </c>
       <c r="D34" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="40"/>
+      <c r="E34" s="40" t="s">
+        <v>302</v>
+      </c>
       <c r="F34" s="41" t="s">
         <v>45</v>
       </c>
       <c r="G34" s="42"/>
       <c r="H34" s="42" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="I34" s="43" t="s">
         <v>4</v>
@@ -4926,912 +5110,866 @@
       <c r="Q34" s="17"/>
     </row>
     <row r="35" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="204"/>
-      <c r="B35" s="235"/>
+      <c r="A35" s="215"/>
+      <c r="B35" s="212"/>
       <c r="C35" s="45">
-        <v>25</v>
-      </c>
-      <c r="D35" s="40" t="s">
-        <v>227</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D35" s="40"/>
       <c r="E35" s="40"/>
-      <c r="F35" s="41" t="s">
-        <v>231</v>
-      </c>
+      <c r="F35" s="50"/>
       <c r="G35" s="43"/>
       <c r="H35" s="43"/>
-      <c r="I35" s="43" t="s">
-        <v>241</v>
-      </c>
+      <c r="I35" s="43"/>
       <c r="J35" s="43"/>
       <c r="K35" s="43"/>
-      <c r="L35" s="44">
-        <v>1</v>
-      </c>
-      <c r="M35" s="117" t="s">
-        <v>267</v>
-      </c>
+      <c r="L35" s="44"/>
+      <c r="M35" s="117"/>
       <c r="N35" s="118"/>
       <c r="O35" s="17"/>
       <c r="P35" s="17"/>
       <c r="Q35" s="17"/>
     </row>
     <row r="36" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="204"/>
-      <c r="B36" s="235"/>
+      <c r="A36" s="215"/>
+      <c r="B36" s="212"/>
       <c r="C36" s="45">
-        <v>26</v>
-      </c>
-      <c r="D36" s="40" t="s">
-        <v>228</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D36" s="40"/>
       <c r="E36" s="40"/>
-      <c r="F36" s="50" t="s">
-        <v>232</v>
-      </c>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43" t="s">
-        <v>241</v>
-      </c>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="43"/>
       <c r="J36" s="43"/>
       <c r="K36" s="43"/>
-      <c r="L36" s="44">
-        <v>1</v>
-      </c>
-      <c r="M36" s="192" t="s">
-        <v>268</v>
-      </c>
+      <c r="L36" s="56"/>
+      <c r="M36" s="117"/>
       <c r="N36" s="118"/>
       <c r="O36" s="17"/>
       <c r="P36" s="17"/>
       <c r="Q36" s="17"/>
     </row>
     <row r="37" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="204"/>
-      <c r="B37" s="235"/>
+      <c r="A37" s="215"/>
+      <c r="B37" s="212"/>
       <c r="C37" s="45">
-        <v>27</v>
-      </c>
-      <c r="D37" s="40" t="s">
-        <v>229</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D37" s="40"/>
       <c r="E37" s="40"/>
-      <c r="F37" s="50" t="s">
-        <v>233</v>
-      </c>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43" t="s">
-        <v>241</v>
-      </c>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="43"/>
       <c r="J37" s="43"/>
       <c r="K37" s="43"/>
-      <c r="L37" s="44">
-        <v>1</v>
-      </c>
-      <c r="M37" s="192" t="s">
-        <v>269</v>
-      </c>
-      <c r="N37" s="118"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="223"/>
+      <c r="N37" s="224"/>
       <c r="O37" s="17"/>
       <c r="P37" s="17"/>
       <c r="Q37" s="17"/>
     </row>
-    <row r="38" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="204"/>
-      <c r="B38" s="235"/>
-      <c r="C38" s="45">
-        <v>28</v>
-      </c>
-      <c r="D38" s="40" t="s">
-        <v>230</v>
-      </c>
-      <c r="E38" s="40"/>
-      <c r="F38" s="50" t="s">
-        <v>234</v>
-      </c>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43" t="s">
-        <v>241</v>
-      </c>
-      <c r="J38" s="43"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="44">
-        <v>1</v>
-      </c>
-      <c r="M38" s="192" t="s">
-        <v>270</v>
-      </c>
-      <c r="N38" s="118"/>
+    <row r="38" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="216"/>
+      <c r="B38" s="213"/>
+      <c r="C38" s="57">
+        <v>32</v>
+      </c>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="91"/>
+      <c r="M38" s="227"/>
+      <c r="N38" s="228"/>
       <c r="O38" s="17"/>
       <c r="P38" s="17"/>
       <c r="Q38" s="17"/>
     </row>
     <row r="39" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="204"/>
-      <c r="B39" s="235"/>
-      <c r="C39" s="45">
-        <v>29</v>
-      </c>
-      <c r="D39" s="40"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="A39" s="214"/>
+      <c r="B39" s="211" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="33">
+        <v>1</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="F39" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="J39" s="43" t="s">
+        <v>4</v>
+      </c>
       <c r="K39" s="43"/>
-      <c r="L39" s="44"/>
-      <c r="M39" s="117"/>
-      <c r="N39" s="118"/>
+      <c r="L39" s="61" t="s">
+        <v>204</v>
+      </c>
+      <c r="M39" s="229"/>
+      <c r="N39" s="230"/>
       <c r="O39" s="17"/>
       <c r="P39" s="17"/>
       <c r="Q39" s="17"/>
     </row>
     <row r="40" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="204"/>
-      <c r="B40" s="235"/>
+      <c r="A40" s="215"/>
+      <c r="B40" s="212"/>
       <c r="C40" s="45">
-        <v>30</v>
-      </c>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="50"/>
+        <v>2</v>
+      </c>
+      <c r="D40" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="F40" s="50" t="s">
+        <v>44</v>
+      </c>
       <c r="G40" s="50"/>
       <c r="H40" s="50"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="43"/>
+      <c r="I40" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="J40" s="43" t="s">
+        <v>4</v>
+      </c>
       <c r="K40" s="43"/>
-      <c r="L40" s="56"/>
-      <c r="M40" s="117"/>
-      <c r="N40" s="118"/>
+      <c r="L40" s="61" t="s">
+        <v>205</v>
+      </c>
+      <c r="M40" s="186"/>
+      <c r="N40" s="187"/>
       <c r="O40" s="17"/>
       <c r="P40" s="17"/>
       <c r="Q40" s="17"/>
     </row>
     <row r="41" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="204"/>
-      <c r="B41" s="235"/>
-      <c r="C41" s="45">
-        <v>31</v>
-      </c>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="50"/>
+      <c r="A41" s="215"/>
+      <c r="B41" s="212"/>
+      <c r="C41" s="191">
+        <v>3</v>
+      </c>
+      <c r="D41" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="F41" s="50" t="s">
+        <v>65</v>
+      </c>
       <c r="G41" s="50"/>
       <c r="H41" s="50"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="43"/>
+      <c r="I41" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="J41" s="43" t="s">
+        <v>4</v>
+      </c>
       <c r="K41" s="43"/>
-      <c r="L41" s="56"/>
-      <c r="M41" s="253"/>
-      <c r="N41" s="254"/>
+      <c r="L41" s="61">
+        <v>1</v>
+      </c>
+      <c r="M41" s="223" t="s">
+        <v>207</v>
+      </c>
+      <c r="N41" s="224"/>
       <c r="O41" s="17"/>
       <c r="P41" s="17"/>
       <c r="Q41" s="17"/>
     </row>
-    <row r="42" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="205"/>
-      <c r="B42" s="236"/>
-      <c r="C42" s="57">
-        <v>32</v>
-      </c>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="60"/>
-      <c r="J42" s="60"/>
-      <c r="K42" s="60"/>
-      <c r="L42" s="91"/>
-      <c r="M42" s="255"/>
-      <c r="N42" s="256"/>
+    <row r="42" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="215"/>
+      <c r="B42" s="212"/>
+      <c r="C42" s="39">
+        <v>4</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="E42" s="40" t="s">
+        <v>306</v>
+      </c>
+      <c r="F42" s="41" t="s">
+        <v>325</v>
+      </c>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="J42" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="K42" s="43"/>
+      <c r="L42" s="44">
+        <v>1</v>
+      </c>
+      <c r="M42" s="192" t="s">
+        <v>259</v>
+      </c>
+      <c r="N42" s="189"/>
       <c r="O42" s="17"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="17"/>
     </row>
-    <row r="43" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="203" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="193" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="33">
-        <v>1</v>
+    <row r="43" spans="1:17" s="55" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="215"/>
+      <c r="B43" s="212"/>
+      <c r="C43" s="39">
+        <v>5</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="40"/>
-      <c r="F43" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="G43" s="50"/>
-      <c r="H43" s="50"/>
+        <v>230</v>
+      </c>
+      <c r="E43" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="F43" s="41" t="s">
+        <v>328</v>
+      </c>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
       <c r="I43" s="43" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J43" s="43" t="s">
         <v>4</v>
       </c>
       <c r="K43" s="43"/>
-      <c r="L43" s="61" t="s">
-        <v>204</v>
-      </c>
-      <c r="M43" s="257"/>
-      <c r="N43" s="258"/>
-      <c r="O43" s="17"/>
-      <c r="P43" s="17"/>
-      <c r="Q43" s="17"/>
+      <c r="L43" s="44">
+        <v>1</v>
+      </c>
+      <c r="M43" s="192" t="s">
+        <v>260</v>
+      </c>
+      <c r="N43" s="189"/>
+      <c r="O43" s="54"/>
+      <c r="P43" s="54"/>
+      <c r="Q43" s="54"/>
     </row>
     <row r="44" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="204"/>
-      <c r="B44" s="194"/>
-      <c r="C44" s="45">
-        <v>2</v>
+      <c r="A44" s="215"/>
+      <c r="B44" s="212"/>
+      <c r="C44" s="39">
+        <v>6</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="E44" s="40"/>
-      <c r="F44" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
+        <v>231</v>
+      </c>
+      <c r="E44" s="40" t="s">
+        <v>308</v>
+      </c>
+      <c r="F44" s="41" t="s">
+        <v>327</v>
+      </c>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
       <c r="I44" s="43" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J44" s="43" t="s">
         <v>4</v>
       </c>
       <c r="K44" s="43"/>
-      <c r="L44" s="61" t="s">
-        <v>205</v>
-      </c>
-      <c r="M44" s="186"/>
-      <c r="N44" s="187"/>
+      <c r="L44" s="44">
+        <v>1</v>
+      </c>
+      <c r="M44" s="192" t="s">
+        <v>261</v>
+      </c>
+      <c r="N44" s="189"/>
       <c r="O44" s="17"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="17"/>
     </row>
     <row r="45" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="204"/>
-      <c r="B45" s="194"/>
-      <c r="C45" s="191">
-        <v>3</v>
+      <c r="A45" s="215"/>
+      <c r="B45" s="212"/>
+      <c r="C45" s="39">
+        <v>7</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="E45" s="40"/>
-      <c r="F45" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
+        <v>232</v>
+      </c>
+      <c r="E45" s="40" t="s">
+        <v>309</v>
+      </c>
+      <c r="F45" s="41" t="s">
+        <v>326</v>
+      </c>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
       <c r="I45" s="43" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J45" s="43" t="s">
         <v>4</v>
       </c>
       <c r="K45" s="43"/>
-      <c r="L45" s="61">
+      <c r="L45" s="44">
         <v>1</v>
       </c>
-      <c r="M45" s="253" t="s">
-        <v>207</v>
-      </c>
-      <c r="N45" s="254"/>
+      <c r="M45" s="192" t="s">
+        <v>262</v>
+      </c>
+      <c r="N45" s="193"/>
       <c r="O45" s="17"/>
       <c r="P45" s="17"/>
       <c r="Q45" s="17"/>
     </row>
     <row r="46" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="204"/>
-      <c r="B46" s="194"/>
+      <c r="A46" s="215"/>
+      <c r="B46" s="212"/>
       <c r="C46" s="39">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="E46" s="40"/>
+        <v>317</v>
+      </c>
+      <c r="E46" s="40" t="s">
+        <v>321</v>
+      </c>
       <c r="F46" s="41" t="s">
-        <v>231</v>
+        <v>329</v>
       </c>
       <c r="G46" s="43"/>
       <c r="H46" s="43"/>
       <c r="I46" s="43" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J46" s="43" t="s">
         <v>4</v>
       </c>
       <c r="K46" s="43"/>
-      <c r="L46" s="44">
-        <v>1</v>
-      </c>
+      <c r="L46" s="44"/>
       <c r="M46" s="192" t="s">
-        <v>267</v>
-      </c>
-      <c r="N46" s="189"/>
+        <v>337</v>
+      </c>
+      <c r="N46" s="193"/>
       <c r="O46" s="17"/>
       <c r="P46" s="17"/>
       <c r="Q46" s="17"/>
     </row>
-    <row r="47" spans="1:17" s="55" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="204"/>
-      <c r="B47" s="194"/>
+    <row r="47" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="215"/>
+      <c r="B47" s="212"/>
       <c r="C47" s="39">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="E47" s="40"/>
-      <c r="F47" s="50" t="s">
-        <v>232</v>
+        <v>318</v>
+      </c>
+      <c r="E47" s="40" t="s">
+        <v>322</v>
+      </c>
+      <c r="F47" s="41" t="s">
+        <v>330</v>
       </c>
       <c r="G47" s="43"/>
       <c r="H47" s="43"/>
       <c r="I47" s="43" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J47" s="43" t="s">
         <v>4</v>
       </c>
       <c r="K47" s="43"/>
-      <c r="L47" s="44">
-        <v>1</v>
-      </c>
+      <c r="L47" s="44"/>
       <c r="M47" s="192" t="s">
-        <v>268</v>
-      </c>
-      <c r="N47" s="189"/>
-      <c r="O47" s="54"/>
-      <c r="P47" s="54"/>
-      <c r="Q47" s="54"/>
+        <v>338</v>
+      </c>
+      <c r="N47" s="193"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="17"/>
     </row>
     <row r="48" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="204"/>
-      <c r="B48" s="194"/>
-      <c r="C48" s="45">
-        <v>6</v>
+      <c r="A48" s="215"/>
+      <c r="B48" s="212"/>
+      <c r="C48" s="39">
+        <v>10</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>239</v>
-      </c>
-      <c r="E48" s="40"/>
-      <c r="F48" s="50" t="s">
-        <v>233</v>
+        <v>319</v>
+      </c>
+      <c r="E48" s="40" t="s">
+        <v>323</v>
+      </c>
+      <c r="F48" s="41" t="s">
+        <v>331</v>
       </c>
       <c r="G48" s="43"/>
       <c r="H48" s="43"/>
       <c r="I48" s="43" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J48" s="43" t="s">
         <v>4</v>
       </c>
       <c r="K48" s="43"/>
-      <c r="L48" s="44">
-        <v>1</v>
-      </c>
+      <c r="L48" s="44"/>
       <c r="M48" s="192" t="s">
-        <v>269</v>
-      </c>
-      <c r="N48" s="189"/>
+        <v>339</v>
+      </c>
+      <c r="N48" s="193"/>
       <c r="O48" s="17"/>
       <c r="P48" s="17"/>
       <c r="Q48" s="17"/>
     </row>
-    <row r="49" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="205"/>
-      <c r="B49" s="195"/>
-      <c r="C49" s="57">
-        <v>7</v>
+    <row r="49" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="215"/>
+      <c r="B49" s="212"/>
+      <c r="C49" s="39">
+        <v>11</v>
       </c>
       <c r="D49" s="40" t="s">
-        <v>240</v>
-      </c>
-      <c r="E49" s="40"/>
-      <c r="F49" s="50" t="s">
-        <v>234</v>
+        <v>320</v>
+      </c>
+      <c r="E49" s="40" t="s">
+        <v>324</v>
+      </c>
+      <c r="F49" s="41" t="s">
+        <v>332</v>
       </c>
       <c r="G49" s="43"/>
       <c r="H49" s="43"/>
       <c r="I49" s="43" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="J49" s="43" t="s">
         <v>4</v>
       </c>
       <c r="K49" s="43"/>
-      <c r="L49" s="44">
-        <v>1</v>
-      </c>
+      <c r="L49" s="44"/>
       <c r="M49" s="192" t="s">
-        <v>270</v>
-      </c>
-      <c r="N49" s="189"/>
+        <v>340</v>
+      </c>
+      <c r="N49" s="193"/>
       <c r="O49" s="17"/>
       <c r="P49" s="17"/>
       <c r="Q49" s="17"/>
     </row>
     <row r="50" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="198" t="s">
-        <v>18</v>
-      </c>
-      <c r="B50" s="200" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" s="69">
-        <v>1</v>
-      </c>
-      <c r="D50" s="93" t="s">
-        <v>40</v>
-      </c>
-      <c r="E50" s="268"/>
-      <c r="F50" s="94" t="s">
-        <v>92</v>
-      </c>
-      <c r="G50" s="92"/>
-      <c r="H50" s="275" t="s">
-        <v>279</v>
-      </c>
-      <c r="I50" s="276" t="s">
-        <v>7</v>
-      </c>
-      <c r="J50" s="276" t="s">
-        <v>6</v>
-      </c>
-      <c r="K50" s="276" t="s">
-        <v>2</v>
-      </c>
-      <c r="L50" s="277" t="s">
-        <v>280</v>
-      </c>
-      <c r="M50" s="196"/>
-      <c r="N50" s="197"/>
+      <c r="A50" s="215"/>
+      <c r="B50" s="212"/>
+      <c r="C50" s="39">
+        <v>12</v>
+      </c>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="44"/>
+      <c r="M50" s="192"/>
+      <c r="N50" s="193"/>
       <c r="O50" s="17"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="17"/>
     </row>
     <row r="51" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="199"/>
-      <c r="B51" s="201"/>
-      <c r="C51" s="67">
-        <v>2</v>
-      </c>
-      <c r="D51" s="262" t="s">
-        <v>86</v>
-      </c>
-      <c r="E51" s="269"/>
-      <c r="F51" s="263" t="s">
-        <v>28</v>
-      </c>
-      <c r="G51" s="264"/>
-      <c r="H51" s="265"/>
-      <c r="I51" s="265" t="s">
-        <v>7</v>
-      </c>
-      <c r="J51" s="265" t="s">
-        <v>6</v>
-      </c>
-      <c r="K51" s="265" t="s">
-        <v>108</v>
-      </c>
-      <c r="L51" s="266" t="s">
-        <v>211</v>
-      </c>
-      <c r="M51" s="267" t="s">
-        <v>285</v>
-      </c>
-      <c r="N51" s="176" t="s">
-        <v>215</v>
-      </c>
+      <c r="A51" s="215"/>
+      <c r="B51" s="212"/>
+      <c r="C51" s="39">
+        <v>13</v>
+      </c>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="44"/>
+      <c r="M51" s="192"/>
+      <c r="N51" s="193"/>
       <c r="O51" s="17"/>
       <c r="P51" s="17"/>
       <c r="Q51" s="17"/>
     </row>
     <row r="52" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="199"/>
-      <c r="B52" s="201"/>
-      <c r="C52" s="69">
-        <v>3</v>
-      </c>
-      <c r="D52" s="62" t="s">
-        <v>87</v>
-      </c>
-      <c r="E52" s="270"/>
-      <c r="F52" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="G52" s="64"/>
-      <c r="H52" s="278" t="s">
-        <v>287</v>
-      </c>
-      <c r="I52" s="279" t="s">
-        <v>7</v>
-      </c>
-      <c r="J52" s="279" t="s">
-        <v>6</v>
-      </c>
-      <c r="K52" s="279" t="s">
-        <v>108</v>
-      </c>
-      <c r="L52" s="280" t="s">
-        <v>210</v>
-      </c>
-      <c r="M52" s="68" t="s">
-        <v>104</v>
-      </c>
-      <c r="N52" s="176" t="s">
-        <v>216</v>
-      </c>
+      <c r="A52" s="215"/>
+      <c r="B52" s="212"/>
+      <c r="C52" s="39">
+        <v>14</v>
+      </c>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="43"/>
+      <c r="J52" s="43"/>
+      <c r="K52" s="43"/>
+      <c r="L52" s="44"/>
+      <c r="M52" s="192"/>
+      <c r="N52" s="193"/>
       <c r="O52" s="17"/>
       <c r="P52" s="17"/>
       <c r="Q52" s="17"/>
     </row>
     <row r="53" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="199"/>
-      <c r="B53" s="201"/>
-      <c r="C53" s="67">
-        <v>4</v>
-      </c>
-      <c r="D53" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="E53" s="270"/>
-      <c r="F53" s="63" t="s">
-        <v>167</v>
-      </c>
-      <c r="G53" s="64"/>
-      <c r="H53" s="278" t="s">
-        <v>288</v>
-      </c>
-      <c r="I53" s="279" t="s">
-        <v>7</v>
-      </c>
-      <c r="J53" s="279" t="s">
-        <v>6</v>
-      </c>
-      <c r="K53" s="279" t="s">
-        <v>108</v>
-      </c>
-      <c r="L53" s="280" t="s">
-        <v>210</v>
-      </c>
-      <c r="M53" s="70" t="s">
-        <v>105</v>
-      </c>
-      <c r="N53" s="177" t="s">
-        <v>217</v>
-      </c>
+      <c r="A53" s="215"/>
+      <c r="B53" s="212"/>
+      <c r="C53" s="39">
+        <v>15</v>
+      </c>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="43"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="44"/>
+      <c r="M53" s="192"/>
+      <c r="N53" s="193"/>
       <c r="O53" s="17"/>
       <c r="P53" s="17"/>
       <c r="Q53" s="17"/>
     </row>
-    <row r="54" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="199"/>
-      <c r="B54" s="201"/>
-      <c r="C54" s="69">
-        <v>5</v>
-      </c>
-      <c r="D54" s="262" t="s">
-        <v>89</v>
-      </c>
-      <c r="E54" s="269"/>
-      <c r="F54" s="263" t="s">
-        <v>28</v>
-      </c>
-      <c r="G54" s="264"/>
-      <c r="H54" s="265"/>
-      <c r="I54" s="265" t="s">
-        <v>7</v>
-      </c>
-      <c r="J54" s="265" t="s">
-        <v>6</v>
-      </c>
-      <c r="K54" s="265" t="s">
-        <v>108</v>
-      </c>
-      <c r="L54" s="266" t="s">
-        <v>211</v>
-      </c>
-      <c r="M54" s="267" t="s">
-        <v>285</v>
-      </c>
-      <c r="N54" s="176" t="s">
-        <v>215</v>
-      </c>
+    <row r="54" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="216"/>
+      <c r="B54" s="213"/>
+      <c r="C54" s="39">
+        <v>16</v>
+      </c>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="43"/>
+      <c r="I54" s="43"/>
+      <c r="J54" s="43"/>
+      <c r="K54" s="43"/>
+      <c r="L54" s="44"/>
+      <c r="M54" s="192"/>
+      <c r="N54" s="193"/>
       <c r="O54" s="17"/>
       <c r="P54" s="17"/>
       <c r="Q54" s="17"/>
     </row>
     <row r="55" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="199"/>
-      <c r="B55" s="201"/>
-      <c r="C55" s="67">
+      <c r="A55" s="219" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="217" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="69">
+        <v>1</v>
+      </c>
+      <c r="D55" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="200" t="s">
+        <v>310</v>
+      </c>
+      <c r="F55" s="94" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" s="92"/>
+      <c r="H55" s="205" t="s">
+        <v>267</v>
+      </c>
+      <c r="I55" s="206" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" s="206" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="E55" s="270"/>
-      <c r="F55" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="G55" s="64"/>
-      <c r="H55" s="278" t="s">
-        <v>289</v>
-      </c>
-      <c r="I55" s="279" t="s">
-        <v>7</v>
-      </c>
-      <c r="J55" s="279" t="s">
-        <v>6</v>
-      </c>
-      <c r="K55" s="279" t="s">
-        <v>108</v>
-      </c>
-      <c r="L55" s="280" t="s">
-        <v>210</v>
-      </c>
-      <c r="M55" s="68" t="s">
-        <v>104</v>
-      </c>
-      <c r="N55" s="176" t="s">
-        <v>216</v>
-      </c>
+      <c r="K55" s="206" t="s">
+        <v>2</v>
+      </c>
+      <c r="L55" s="207" t="s">
+        <v>268</v>
+      </c>
+      <c r="M55" s="263"/>
+      <c r="N55" s="264"/>
       <c r="O55" s="17"/>
       <c r="P55" s="17"/>
       <c r="Q55" s="17"/>
     </row>
-    <row r="56" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="199"/>
-      <c r="B56" s="201"/>
-      <c r="C56" s="69">
+    <row r="56" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="220"/>
+      <c r="B56" s="218"/>
+      <c r="C56" s="67">
+        <v>2</v>
+      </c>
+      <c r="D56" s="194" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" s="201"/>
+      <c r="F56" s="195" t="s">
+        <v>28</v>
+      </c>
+      <c r="G56" s="196"/>
+      <c r="H56" s="197"/>
+      <c r="I56" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="D56" s="62" t="s">
-        <v>91</v>
-      </c>
-      <c r="E56" s="270"/>
-      <c r="F56" s="63" t="s">
-        <v>167</v>
-      </c>
-      <c r="G56" s="64"/>
-      <c r="H56" s="278" t="s">
-        <v>290</v>
-      </c>
-      <c r="I56" s="279" t="s">
-        <v>7</v>
-      </c>
-      <c r="J56" s="279" t="s">
+      <c r="J56" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="K56" s="279" t="s">
+      <c r="K56" s="197" t="s">
         <v>108</v>
       </c>
-      <c r="L56" s="280" t="s">
-        <v>210</v>
-      </c>
-      <c r="M56" s="70" t="s">
-        <v>105</v>
-      </c>
-      <c r="N56" s="177" t="s">
-        <v>217</v>
+      <c r="L56" s="198" t="s">
+        <v>211</v>
+      </c>
+      <c r="M56" s="199" t="s">
+        <v>273</v>
+      </c>
+      <c r="N56" s="176" t="s">
+        <v>215</v>
       </c>
       <c r="O56" s="17"/>
       <c r="P56" s="17"/>
       <c r="Q56" s="17"/>
     </row>
-    <row r="57" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="199"/>
-      <c r="B57" s="201"/>
-      <c r="C57" s="67">
-        <v>8</v>
+    <row r="57" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="220"/>
+      <c r="B57" s="218"/>
+      <c r="C57" s="69">
+        <v>3</v>
       </c>
       <c r="D57" s="62" t="s">
-        <v>84</v>
-      </c>
-      <c r="E57" s="270"/>
+        <v>87</v>
+      </c>
+      <c r="E57" s="200" t="s">
+        <v>311</v>
+      </c>
       <c r="F57" s="63" t="s">
-        <v>29</v>
+        <v>166</v>
       </c>
       <c r="G57" s="64"/>
-      <c r="H57" s="65" t="s">
-        <v>281</v>
-      </c>
-      <c r="I57" s="65" t="s">
+      <c r="H57" s="208" t="s">
+        <v>274</v>
+      </c>
+      <c r="I57" s="209" t="s">
         <v>7</v>
       </c>
-      <c r="J57" s="65" t="s">
+      <c r="J57" s="209" t="s">
         <v>6</v>
       </c>
-      <c r="K57" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="L57" s="71" t="s">
-        <v>209</v>
-      </c>
-      <c r="M57" s="251" t="s">
-        <v>51</v>
-      </c>
-      <c r="N57" s="252"/>
+      <c r="K57" s="209" t="s">
+        <v>108</v>
+      </c>
+      <c r="L57" s="210" t="s">
+        <v>210</v>
+      </c>
+      <c r="M57" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="N57" s="176" t="s">
+        <v>216</v>
+      </c>
       <c r="O57" s="17"/>
       <c r="P57" s="17"/>
       <c r="Q57" s="17"/>
     </row>
-    <row r="58" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="199"/>
-      <c r="B58" s="201"/>
-      <c r="C58" s="69">
-        <v>9</v>
+    <row r="58" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="220"/>
+      <c r="B58" s="218"/>
+      <c r="C58" s="67">
+        <v>4</v>
       </c>
       <c r="D58" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="E58" s="270"/>
+        <v>88</v>
+      </c>
+      <c r="E58" s="200" t="s">
+        <v>312</v>
+      </c>
       <c r="F58" s="63" t="s">
-        <v>29</v>
+        <v>167</v>
       </c>
       <c r="G58" s="64"/>
-      <c r="H58" s="65" t="s">
-        <v>282</v>
-      </c>
-      <c r="I58" s="65" t="s">
+      <c r="H58" s="208" t="s">
+        <v>275</v>
+      </c>
+      <c r="I58" s="209" t="s">
         <v>7</v>
       </c>
-      <c r="J58" s="65" t="s">
+      <c r="J58" s="209" t="s">
         <v>6</v>
       </c>
-      <c r="K58" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="L58" s="71" t="s">
-        <v>209</v>
-      </c>
-      <c r="M58" s="251" t="s">
-        <v>51</v>
-      </c>
-      <c r="N58" s="252"/>
-      <c r="O58" s="73"/>
-      <c r="P58" s="73"/>
-      <c r="Q58" s="73"/>
-    </row>
-    <row r="59" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="199"/>
-      <c r="B59" s="201"/>
-      <c r="C59" s="67">
-        <v>10</v>
-      </c>
-      <c r="D59" s="62" t="s">
-        <v>199</v>
-      </c>
-      <c r="E59" s="270"/>
-      <c r="F59" s="63" t="s">
-        <v>201</v>
-      </c>
-      <c r="G59" s="64"/>
-      <c r="H59" s="279" t="s">
-        <v>283</v>
-      </c>
-      <c r="I59" s="279" t="s">
+      <c r="K58" s="209" t="s">
+        <v>108</v>
+      </c>
+      <c r="L58" s="210" t="s">
+        <v>210</v>
+      </c>
+      <c r="M58" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="N58" s="177" t="s">
+        <v>217</v>
+      </c>
+      <c r="O58" s="17"/>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17"/>
+    </row>
+    <row r="59" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="220"/>
+      <c r="B59" s="218"/>
+      <c r="C59" s="69">
+        <v>5</v>
+      </c>
+      <c r="D59" s="194" t="s">
+        <v>89</v>
+      </c>
+      <c r="E59" s="201"/>
+      <c r="F59" s="195" t="s">
+        <v>28</v>
+      </c>
+      <c r="G59" s="196"/>
+      <c r="H59" s="197"/>
+      <c r="I59" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="J59" s="279" t="s">
+      <c r="J59" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="K59" s="279" t="s">
-        <v>2</v>
-      </c>
-      <c r="L59" s="280" t="s">
-        <v>208</v>
-      </c>
-      <c r="M59" s="208" t="s">
-        <v>198</v>
-      </c>
-      <c r="N59" s="209"/>
+      <c r="K59" s="197" t="s">
+        <v>108</v>
+      </c>
+      <c r="L59" s="198" t="s">
+        <v>211</v>
+      </c>
+      <c r="M59" s="199" t="s">
+        <v>273</v>
+      </c>
+      <c r="N59" s="176" t="s">
+        <v>215</v>
+      </c>
       <c r="O59" s="73"/>
       <c r="P59" s="73"/>
       <c r="Q59" s="73"/>
     </row>
-    <row r="60" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="199"/>
-      <c r="B60" s="201"/>
-      <c r="C60" s="69">
-        <v>11</v>
+    <row r="60" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="220"/>
+      <c r="B60" s="218"/>
+      <c r="C60" s="67">
+        <v>6</v>
       </c>
       <c r="D60" s="62" t="s">
-        <v>200</v>
-      </c>
-      <c r="E60" s="270"/>
+        <v>90</v>
+      </c>
+      <c r="E60" s="200" t="s">
+        <v>313</v>
+      </c>
       <c r="F60" s="63" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
       <c r="G60" s="64"/>
-      <c r="H60" s="279" t="s">
-        <v>284</v>
-      </c>
-      <c r="I60" s="279" t="s">
+      <c r="H60" s="208" t="s">
+        <v>276</v>
+      </c>
+      <c r="I60" s="209" t="s">
         <v>7</v>
       </c>
-      <c r="J60" s="279" t="s">
+      <c r="J60" s="209" t="s">
         <v>6</v>
       </c>
-      <c r="K60" s="279" t="s">
-        <v>2</v>
-      </c>
-      <c r="L60" s="280" t="s">
-        <v>208</v>
-      </c>
-      <c r="M60" s="208" t="s">
-        <v>198</v>
-      </c>
-      <c r="N60" s="209"/>
+      <c r="K60" s="209" t="s">
+        <v>108</v>
+      </c>
+      <c r="L60" s="210" t="s">
+        <v>210</v>
+      </c>
+      <c r="M60" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="N60" s="176" t="s">
+        <v>216</v>
+      </c>
       <c r="O60" s="73"/>
       <c r="P60" s="73"/>
       <c r="Q60" s="73"/>
     </row>
     <row r="61" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="199"/>
-      <c r="B61" s="201"/>
-      <c r="C61" s="67">
-        <v>12</v>
+      <c r="A61" s="220"/>
+      <c r="B61" s="218"/>
+      <c r="C61" s="69">
+        <v>7</v>
       </c>
       <c r="D61" s="62" t="s">
-        <v>171</v>
-      </c>
-      <c r="E61" s="270"/>
-      <c r="F61" s="72" t="s">
-        <v>168</v>
+        <v>91</v>
+      </c>
+      <c r="E61" s="200" t="s">
+        <v>314</v>
+      </c>
+      <c r="F61" s="63" t="s">
+        <v>167</v>
       </c>
       <c r="G61" s="64"/>
-      <c r="H61" s="64" t="s">
-        <v>276</v>
-      </c>
-      <c r="I61" s="65" t="s">
+      <c r="H61" s="208" t="s">
+        <v>277</v>
+      </c>
+      <c r="I61" s="209" t="s">
         <v>7</v>
       </c>
-      <c r="J61" s="65" t="s">
+      <c r="J61" s="209" t="s">
         <v>6</v>
       </c>
-      <c r="K61" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="L61" s="66" t="s">
-        <v>206</v>
-      </c>
-      <c r="M61" s="210"/>
-      <c r="N61" s="211"/>
+      <c r="K61" s="209" t="s">
+        <v>108</v>
+      </c>
+      <c r="L61" s="210" t="s">
+        <v>210</v>
+      </c>
+      <c r="M61" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="N61" s="177" t="s">
+        <v>217</v>
+      </c>
       <c r="O61" s="73"/>
       <c r="P61" s="73"/>
       <c r="Q61" s="73"/>
     </row>
     <row r="62" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="199"/>
-      <c r="B62" s="201"/>
-      <c r="C62" s="69">
-        <v>13</v>
+      <c r="A62" s="220"/>
+      <c r="B62" s="218"/>
+      <c r="C62" s="67">
+        <v>8</v>
       </c>
       <c r="D62" s="62" t="s">
-        <v>172</v>
-      </c>
-      <c r="E62" s="270"/>
-      <c r="F62" s="72" t="s">
-        <v>169</v>
+        <v>84</v>
+      </c>
+      <c r="E62" s="202" t="s">
+        <v>315</v>
+      </c>
+      <c r="F62" s="63" t="s">
+        <v>29</v>
       </c>
       <c r="G62" s="64"/>
-      <c r="H62" s="64" t="s">
-        <v>277</v>
+      <c r="H62" s="65" t="s">
+        <v>269</v>
       </c>
       <c r="I62" s="65" t="s">
         <v>7</v>
@@ -5840,33 +5978,37 @@
         <v>6</v>
       </c>
       <c r="K62" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="L62" s="66" t="s">
-        <v>206</v>
-      </c>
-      <c r="M62" s="210"/>
-      <c r="N62" s="211"/>
+        <v>2</v>
+      </c>
+      <c r="L62" s="71" t="s">
+        <v>209</v>
+      </c>
+      <c r="M62" s="221" t="s">
+        <v>51</v>
+      </c>
+      <c r="N62" s="222"/>
       <c r="O62" s="73"/>
       <c r="P62" s="73"/>
       <c r="Q62" s="73"/>
     </row>
     <row r="63" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="199"/>
-      <c r="B63" s="201"/>
-      <c r="C63" s="67">
-        <v>14</v>
+      <c r="A63" s="220"/>
+      <c r="B63" s="218"/>
+      <c r="C63" s="69">
+        <v>9</v>
       </c>
       <c r="D63" s="62" t="s">
-        <v>173</v>
-      </c>
-      <c r="E63" s="270"/>
-      <c r="F63" s="72" t="s">
-        <v>170</v>
+        <v>85</v>
+      </c>
+      <c r="E63" s="202" t="s">
+        <v>316</v>
+      </c>
+      <c r="F63" s="63" t="s">
+        <v>29</v>
       </c>
       <c r="G63" s="64"/>
-      <c r="H63" s="64" t="s">
-        <v>278</v>
+      <c r="H63" s="65" t="s">
+        <v>270</v>
       </c>
       <c r="I63" s="65" t="s">
         <v>7</v>
@@ -5875,193 +6017,269 @@
         <v>6</v>
       </c>
       <c r="K63" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="L63" s="66" t="s">
-        <v>206</v>
-      </c>
-      <c r="M63" s="212"/>
-      <c r="N63" s="213"/>
+        <v>2</v>
+      </c>
+      <c r="L63" s="71" t="s">
+        <v>209</v>
+      </c>
+      <c r="M63" s="221" t="s">
+        <v>51</v>
+      </c>
+      <c r="N63" s="222"/>
       <c r="O63" s="73"/>
       <c r="P63" s="73"/>
       <c r="Q63" s="73"/>
     </row>
     <row r="64" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="199"/>
-      <c r="B64" s="201"/>
-      <c r="C64" s="69">
-        <v>15</v>
-      </c>
-      <c r="D64" s="62"/>
-      <c r="E64" s="270"/>
-      <c r="F64" s="63"/>
+      <c r="A64" s="220"/>
+      <c r="B64" s="218"/>
+      <c r="C64" s="67">
+        <v>10</v>
+      </c>
+      <c r="D64" s="62" t="s">
+        <v>199</v>
+      </c>
+      <c r="E64" s="202"/>
+      <c r="F64" s="63" t="s">
+        <v>201</v>
+      </c>
       <c r="G64" s="64"/>
-      <c r="H64" s="65"/>
-      <c r="I64" s="65"/>
-      <c r="J64" s="65"/>
-      <c r="K64" s="65"/>
-      <c r="L64" s="66"/>
-      <c r="M64" s="210"/>
-      <c r="N64" s="211"/>
+      <c r="H64" s="209" t="s">
+        <v>271</v>
+      </c>
+      <c r="I64" s="209" t="s">
+        <v>7</v>
+      </c>
+      <c r="J64" s="209" t="s">
+        <v>6</v>
+      </c>
+      <c r="K64" s="209" t="s">
+        <v>2</v>
+      </c>
+      <c r="L64" s="210" t="s">
+        <v>208</v>
+      </c>
+      <c r="M64" s="267" t="s">
+        <v>198</v>
+      </c>
+      <c r="N64" s="268"/>
       <c r="O64" s="73"/>
       <c r="P64" s="73"/>
       <c r="Q64" s="73"/>
     </row>
     <row r="65" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="199"/>
-      <c r="B65" s="201"/>
-      <c r="C65" s="67">
-        <v>16</v>
-      </c>
-      <c r="D65" s="62"/>
-      <c r="E65" s="270"/>
-      <c r="F65" s="63"/>
+      <c r="A65" s="220"/>
+      <c r="B65" s="218"/>
+      <c r="C65" s="69">
+        <v>11</v>
+      </c>
+      <c r="D65" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="E65" s="202"/>
+      <c r="F65" s="63" t="s">
+        <v>201</v>
+      </c>
       <c r="G65" s="64"/>
-      <c r="H65" s="64"/>
-      <c r="I65" s="65"/>
-      <c r="J65" s="65"/>
-      <c r="K65" s="65"/>
-      <c r="L65" s="66"/>
-      <c r="M65" s="210"/>
-      <c r="N65" s="211"/>
+      <c r="H65" s="209" t="s">
+        <v>272</v>
+      </c>
+      <c r="I65" s="209" t="s">
+        <v>7</v>
+      </c>
+      <c r="J65" s="209" t="s">
+        <v>6</v>
+      </c>
+      <c r="K65" s="209" t="s">
+        <v>2</v>
+      </c>
+      <c r="L65" s="210" t="s">
+        <v>208</v>
+      </c>
+      <c r="M65" s="267" t="s">
+        <v>198</v>
+      </c>
+      <c r="N65" s="268"/>
       <c r="O65" s="73"/>
       <c r="P65" s="73"/>
       <c r="Q65" s="73"/>
     </row>
-    <row r="66" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="199"/>
-      <c r="B66" s="201"/>
-      <c r="C66" s="69">
-        <v>17</v>
-      </c>
-      <c r="D66" s="62"/>
-      <c r="E66" s="270"/>
-      <c r="F66" s="63"/>
+    <row r="66" spans="1:17" s="74" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="220"/>
+      <c r="B66" s="218"/>
+      <c r="C66" s="67">
+        <v>12</v>
+      </c>
+      <c r="D66" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="E66" s="202"/>
+      <c r="F66" s="72" t="s">
+        <v>168</v>
+      </c>
       <c r="G66" s="64"/>
-      <c r="H66" s="64"/>
-      <c r="I66" s="65"/>
-      <c r="J66" s="65"/>
-      <c r="K66" s="65"/>
-      <c r="L66" s="66"/>
-      <c r="M66" s="212"/>
-      <c r="N66" s="213"/>
+      <c r="H66" s="64" t="s">
+        <v>264</v>
+      </c>
+      <c r="I66" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="J66" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="K66" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="L66" s="66" t="s">
+        <v>206</v>
+      </c>
+      <c r="M66" s="269"/>
+      <c r="N66" s="270"/>
       <c r="O66" s="73"/>
       <c r="P66" s="73"/>
       <c r="Q66" s="73"/>
     </row>
-    <row r="67" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="199"/>
-      <c r="B67" s="201"/>
-      <c r="C67" s="67">
-        <v>18</v>
-      </c>
-      <c r="D67" s="75"/>
-      <c r="E67" s="271"/>
-      <c r="F67" s="76"/>
-      <c r="G67" s="77"/>
-      <c r="H67" s="77"/>
-      <c r="I67" s="78"/>
-      <c r="J67" s="78"/>
-      <c r="K67" s="78"/>
-      <c r="L67" s="79"/>
-      <c r="M67" s="80"/>
-      <c r="N67" s="81"/>
+    <row r="67" spans="1:17" s="74" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="220"/>
+      <c r="B67" s="218"/>
+      <c r="C67" s="69">
+        <v>13</v>
+      </c>
+      <c r="D67" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="E67" s="202"/>
+      <c r="F67" s="72" t="s">
+        <v>169</v>
+      </c>
+      <c r="G67" s="64"/>
+      <c r="H67" s="64" t="s">
+        <v>265</v>
+      </c>
+      <c r="I67" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="J67" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="K67" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="L67" s="66" t="s">
+        <v>206</v>
+      </c>
+      <c r="M67" s="269"/>
+      <c r="N67" s="270"/>
       <c r="O67" s="73"/>
       <c r="P67" s="73"/>
       <c r="Q67" s="73"/>
     </row>
-    <row r="68" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="199"/>
-      <c r="B68" s="201"/>
-      <c r="C68" s="69">
-        <v>19</v>
-      </c>
-      <c r="D68" s="62"/>
-      <c r="E68" s="270"/>
-      <c r="F68" s="72"/>
+    <row r="68" spans="1:17" s="74" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="220"/>
+      <c r="B68" s="218"/>
+      <c r="C68" s="67">
+        <v>14</v>
+      </c>
+      <c r="D68" s="62" t="s">
+        <v>173</v>
+      </c>
+      <c r="E68" s="202"/>
+      <c r="F68" s="72" t="s">
+        <v>170</v>
+      </c>
       <c r="G68" s="64"/>
-      <c r="H68" s="64"/>
-      <c r="I68" s="65"/>
-      <c r="J68" s="65"/>
-      <c r="K68" s="65"/>
-      <c r="L68" s="66"/>
-      <c r="M68" s="80"/>
-      <c r="N68" s="81"/>
+      <c r="H68" s="64" t="s">
+        <v>266</v>
+      </c>
+      <c r="I68" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="J68" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="K68" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="L68" s="66" t="s">
+        <v>206</v>
+      </c>
+      <c r="M68" s="271"/>
+      <c r="N68" s="272"/>
       <c r="O68" s="73"/>
       <c r="P68" s="73"/>
       <c r="Q68" s="73"/>
     </row>
     <row r="69" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="199"/>
-      <c r="B69" s="201"/>
-      <c r="C69" s="67">
-        <v>20</v>
+      <c r="A69" s="220"/>
+      <c r="B69" s="218"/>
+      <c r="C69" s="69">
+        <v>15</v>
       </c>
       <c r="D69" s="62"/>
-      <c r="E69" s="270"/>
-      <c r="F69" s="72"/>
+      <c r="E69" s="202"/>
+      <c r="F69" s="63"/>
       <c r="G69" s="64"/>
-      <c r="H69" s="64"/>
+      <c r="H69" s="65"/>
       <c r="I69" s="65"/>
       <c r="J69" s="65"/>
       <c r="K69" s="65"/>
       <c r="L69" s="66"/>
-      <c r="M69" s="80"/>
-      <c r="N69" s="81"/>
+      <c r="M69" s="269"/>
+      <c r="N69" s="270"/>
       <c r="O69" s="73"/>
       <c r="P69" s="73"/>
       <c r="Q69" s="73"/>
     </row>
     <row r="70" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="199"/>
-      <c r="B70" s="201"/>
-      <c r="C70" s="69">
-        <v>21</v>
+      <c r="A70" s="220"/>
+      <c r="B70" s="218"/>
+      <c r="C70" s="67">
+        <v>16</v>
       </c>
       <c r="D70" s="62"/>
-      <c r="E70" s="270"/>
-      <c r="F70" s="72"/>
+      <c r="E70" s="202"/>
+      <c r="F70" s="63"/>
       <c r="G70" s="64"/>
       <c r="H70" s="64"/>
       <c r="I70" s="65"/>
       <c r="J70" s="65"/>
       <c r="K70" s="65"/>
       <c r="L70" s="66"/>
-      <c r="M70" s="80"/>
-      <c r="N70" s="81"/>
+      <c r="M70" s="269"/>
+      <c r="N70" s="270"/>
       <c r="O70" s="73"/>
       <c r="P70" s="73"/>
       <c r="Q70" s="73"/>
     </row>
     <row r="71" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="199"/>
-      <c r="B71" s="201"/>
-      <c r="C71" s="67">
-        <v>22</v>
-      </c>
-      <c r="D71" s="75"/>
-      <c r="E71" s="271"/>
-      <c r="F71" s="76"/>
-      <c r="G71" s="77"/>
-      <c r="H71" s="77"/>
-      <c r="I71" s="78"/>
-      <c r="J71" s="78"/>
-      <c r="K71" s="78"/>
-      <c r="L71" s="79"/>
-      <c r="M71" s="80"/>
-      <c r="N71" s="81"/>
+      <c r="A71" s="220"/>
+      <c r="B71" s="218"/>
+      <c r="C71" s="69">
+        <v>17</v>
+      </c>
+      <c r="D71" s="62"/>
+      <c r="E71" s="202"/>
+      <c r="F71" s="63"/>
+      <c r="G71" s="64"/>
+      <c r="H71" s="64"/>
+      <c r="I71" s="65"/>
+      <c r="J71" s="65"/>
+      <c r="K71" s="65"/>
+      <c r="L71" s="66"/>
+      <c r="M71" s="271"/>
+      <c r="N71" s="272"/>
       <c r="O71" s="73"/>
       <c r="P71" s="73"/>
       <c r="Q71" s="73"/>
     </row>
     <row r="72" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="199"/>
-      <c r="B72" s="201"/>
-      <c r="C72" s="69">
-        <v>23</v>
+      <c r="A72" s="220"/>
+      <c r="B72" s="218"/>
+      <c r="C72" s="67">
+        <v>18</v>
       </c>
       <c r="D72" s="75"/>
-      <c r="E72" s="271"/>
+      <c r="E72" s="203"/>
       <c r="F72" s="76"/>
       <c r="G72" s="77"/>
       <c r="H72" s="77"/>
@@ -6076,20 +6294,20 @@
       <c r="Q72" s="73"/>
     </row>
     <row r="73" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="199"/>
-      <c r="B73" s="201"/>
-      <c r="C73" s="67">
-        <v>24</v>
-      </c>
-      <c r="D73" s="75"/>
-      <c r="E73" s="271"/>
-      <c r="F73" s="76"/>
-      <c r="G73" s="77"/>
-      <c r="H73" s="77"/>
-      <c r="I73" s="78"/>
-      <c r="J73" s="78"/>
-      <c r="K73" s="78"/>
-      <c r="L73" s="79"/>
+      <c r="A73" s="220"/>
+      <c r="B73" s="218"/>
+      <c r="C73" s="69">
+        <v>19</v>
+      </c>
+      <c r="D73" s="62"/>
+      <c r="E73" s="202"/>
+      <c r="F73" s="72"/>
+      <c r="G73" s="64"/>
+      <c r="H73" s="64"/>
+      <c r="I73" s="65"/>
+      <c r="J73" s="65"/>
+      <c r="K73" s="65"/>
+      <c r="L73" s="66"/>
       <c r="M73" s="80"/>
       <c r="N73" s="81"/>
       <c r="O73" s="73"/>
@@ -6097,20 +6315,20 @@
       <c r="Q73" s="73"/>
     </row>
     <row r="74" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="199"/>
-      <c r="B74" s="201"/>
-      <c r="C74" s="69">
-        <v>25</v>
-      </c>
-      <c r="D74" s="75"/>
-      <c r="E74" s="271"/>
-      <c r="F74" s="76"/>
-      <c r="G74" s="77"/>
-      <c r="H74" s="77"/>
-      <c r="I74" s="78"/>
-      <c r="J74" s="78"/>
-      <c r="K74" s="78"/>
-      <c r="L74" s="79"/>
+      <c r="A74" s="220"/>
+      <c r="B74" s="218"/>
+      <c r="C74" s="67">
+        <v>20</v>
+      </c>
+      <c r="D74" s="62"/>
+      <c r="E74" s="202"/>
+      <c r="F74" s="72"/>
+      <c r="G74" s="64"/>
+      <c r="H74" s="64"/>
+      <c r="I74" s="65"/>
+      <c r="J74" s="65"/>
+      <c r="K74" s="65"/>
+      <c r="L74" s="66"/>
       <c r="M74" s="80"/>
       <c r="N74" s="81"/>
       <c r="O74" s="73"/>
@@ -6118,55 +6336,55 @@
       <c r="Q74" s="73"/>
     </row>
     <row r="75" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="199"/>
-      <c r="B75" s="201"/>
-      <c r="C75" s="67">
-        <v>26</v>
+      <c r="A75" s="220"/>
+      <c r="B75" s="218"/>
+      <c r="C75" s="69">
+        <v>21</v>
       </c>
       <c r="D75" s="62"/>
-      <c r="E75" s="270"/>
-      <c r="F75" s="63"/>
+      <c r="E75" s="202"/>
+      <c r="F75" s="72"/>
       <c r="G75" s="64"/>
-      <c r="H75" s="65"/>
+      <c r="H75" s="64"/>
       <c r="I75" s="65"/>
       <c r="J75" s="65"/>
       <c r="K75" s="65"/>
-      <c r="L75" s="71"/>
-      <c r="M75" s="214"/>
-      <c r="N75" s="215"/>
+      <c r="L75" s="66"/>
+      <c r="M75" s="80"/>
+      <c r="N75" s="81"/>
       <c r="O75" s="73"/>
       <c r="P75" s="73"/>
       <c r="Q75" s="73"/>
     </row>
     <row r="76" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="199"/>
-      <c r="B76" s="201"/>
-      <c r="C76" s="69">
-        <v>27</v>
-      </c>
-      <c r="D76" s="62"/>
-      <c r="E76" s="270"/>
-      <c r="F76" s="63"/>
-      <c r="G76" s="64"/>
-      <c r="H76" s="65"/>
-      <c r="I76" s="65"/>
-      <c r="J76" s="65"/>
-      <c r="K76" s="65"/>
-      <c r="L76" s="71"/>
-      <c r="M76" s="214"/>
-      <c r="N76" s="215"/>
+      <c r="A76" s="220"/>
+      <c r="B76" s="218"/>
+      <c r="C76" s="67">
+        <v>22</v>
+      </c>
+      <c r="D76" s="75"/>
+      <c r="E76" s="203"/>
+      <c r="F76" s="76"/>
+      <c r="G76" s="77"/>
+      <c r="H76" s="77"/>
+      <c r="I76" s="78"/>
+      <c r="J76" s="78"/>
+      <c r="K76" s="78"/>
+      <c r="L76" s="79"/>
+      <c r="M76" s="80"/>
+      <c r="N76" s="81"/>
       <c r="O76" s="73"/>
       <c r="P76" s="73"/>
       <c r="Q76" s="73"/>
     </row>
     <row r="77" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="199"/>
-      <c r="B77" s="201"/>
-      <c r="C77" s="67">
-        <v>28</v>
+      <c r="A77" s="220"/>
+      <c r="B77" s="218"/>
+      <c r="C77" s="69">
+        <v>23</v>
       </c>
       <c r="D77" s="75"/>
-      <c r="E77" s="271"/>
+      <c r="E77" s="203"/>
       <c r="F77" s="76"/>
       <c r="G77" s="77"/>
       <c r="H77" s="77"/>
@@ -6181,13 +6399,13 @@
       <c r="Q77" s="73"/>
     </row>
     <row r="78" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="199"/>
-      <c r="B78" s="201"/>
-      <c r="C78" s="69">
-        <v>29</v>
+      <c r="A78" s="220"/>
+      <c r="B78" s="218"/>
+      <c r="C78" s="67">
+        <v>24</v>
       </c>
       <c r="D78" s="75"/>
-      <c r="E78" s="271"/>
+      <c r="E78" s="203"/>
       <c r="F78" s="76"/>
       <c r="G78" s="77"/>
       <c r="H78" s="77"/>
@@ -6201,14 +6419,14 @@
       <c r="P78" s="73"/>
       <c r="Q78" s="73"/>
     </row>
-    <row r="79" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="199"/>
-      <c r="B79" s="201"/>
-      <c r="C79" s="67">
-        <v>30</v>
+    <row r="79" spans="1:17" s="74" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="220"/>
+      <c r="B79" s="218"/>
+      <c r="C79" s="69">
+        <v>25</v>
       </c>
       <c r="D79" s="75"/>
-      <c r="E79" s="271"/>
+      <c r="E79" s="203"/>
       <c r="F79" s="76"/>
       <c r="G79" s="77"/>
       <c r="H79" s="77"/>
@@ -6218,65 +6436,168 @@
       <c r="L79" s="79"/>
       <c r="M79" s="80"/>
       <c r="N79" s="81"/>
-      <c r="O79" s="17"/>
-      <c r="P79" s="17"/>
-      <c r="Q79" s="17"/>
+      <c r="O79" s="73"/>
+      <c r="P79" s="73"/>
+      <c r="Q79" s="73"/>
     </row>
     <row r="80" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="199"/>
-      <c r="B80" s="201"/>
-      <c r="C80" s="69">
+      <c r="A80" s="220"/>
+      <c r="B80" s="218"/>
+      <c r="C80" s="67">
+        <v>26</v>
+      </c>
+      <c r="D80" s="62"/>
+      <c r="E80" s="202"/>
+      <c r="F80" s="63"/>
+      <c r="G80" s="64"/>
+      <c r="H80" s="65"/>
+      <c r="I80" s="65"/>
+      <c r="J80" s="65"/>
+      <c r="K80" s="65"/>
+      <c r="L80" s="71"/>
+      <c r="M80" s="273"/>
+      <c r="N80" s="274"/>
+      <c r="O80" s="17"/>
+      <c r="P80" s="17"/>
+      <c r="Q80" s="17"/>
+    </row>
+    <row r="81" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="220"/>
+      <c r="B81" s="218"/>
+      <c r="C81" s="69">
+        <v>27</v>
+      </c>
+      <c r="D81" s="62"/>
+      <c r="E81" s="202"/>
+      <c r="F81" s="63"/>
+      <c r="G81" s="64"/>
+      <c r="H81" s="65"/>
+      <c r="I81" s="65"/>
+      <c r="J81" s="65"/>
+      <c r="K81" s="65"/>
+      <c r="L81" s="71"/>
+      <c r="M81" s="273"/>
+      <c r="N81" s="274"/>
+    </row>
+    <row r="82" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="220"/>
+      <c r="B82" s="218"/>
+      <c r="C82" s="67">
+        <v>28</v>
+      </c>
+      <c r="D82" s="75"/>
+      <c r="E82" s="203"/>
+      <c r="F82" s="76"/>
+      <c r="G82" s="77"/>
+      <c r="H82" s="77"/>
+      <c r="I82" s="78"/>
+      <c r="J82" s="78"/>
+      <c r="K82" s="78"/>
+      <c r="L82" s="79"/>
+      <c r="M82" s="80"/>
+      <c r="N82" s="81"/>
+    </row>
+    <row r="83" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="220"/>
+      <c r="B83" s="218"/>
+      <c r="C83" s="69">
+        <v>29</v>
+      </c>
+      <c r="D83" s="75"/>
+      <c r="E83" s="203"/>
+      <c r="F83" s="76"/>
+      <c r="G83" s="77"/>
+      <c r="H83" s="77"/>
+      <c r="I83" s="78"/>
+      <c r="J83" s="78"/>
+      <c r="K83" s="78"/>
+      <c r="L83" s="79"/>
+      <c r="M83" s="80"/>
+      <c r="N83" s="81"/>
+    </row>
+    <row r="84" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="220"/>
+      <c r="B84" s="218"/>
+      <c r="C84" s="67">
+        <v>30</v>
+      </c>
+      <c r="D84" s="75"/>
+      <c r="E84" s="203"/>
+      <c r="F84" s="76"/>
+      <c r="G84" s="77"/>
+      <c r="H84" s="77"/>
+      <c r="I84" s="78"/>
+      <c r="J84" s="78"/>
+      <c r="K84" s="78"/>
+      <c r="L84" s="79"/>
+      <c r="M84" s="80"/>
+      <c r="N84" s="81"/>
+    </row>
+    <row r="85" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="220"/>
+      <c r="B85" s="218"/>
+      <c r="C85" s="69">
         <v>31</v>
       </c>
-      <c r="D80" s="75"/>
-      <c r="E80" s="271"/>
-      <c r="F80" s="76"/>
-      <c r="G80" s="77"/>
-      <c r="H80" s="77"/>
-      <c r="I80" s="78"/>
-      <c r="J80" s="78"/>
-      <c r="K80" s="78"/>
-      <c r="L80" s="79"/>
-      <c r="M80" s="80"/>
-      <c r="N80" s="81"/>
-    </row>
-    <row r="81" spans="1:14" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="199"/>
-      <c r="B81" s="202"/>
-      <c r="C81" s="67">
+      <c r="D85" s="75"/>
+      <c r="E85" s="203"/>
+      <c r="F85" s="76"/>
+      <c r="G85" s="77"/>
+      <c r="H85" s="77"/>
+      <c r="I85" s="78"/>
+      <c r="J85" s="78"/>
+      <c r="K85" s="78"/>
+      <c r="L85" s="79"/>
+      <c r="M85" s="80"/>
+      <c r="N85" s="81"/>
+    </row>
+    <row r="86" spans="1:14" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="220"/>
+      <c r="B86" s="218"/>
+      <c r="C86" s="67">
         <v>32</v>
       </c>
-      <c r="D81" s="82"/>
-      <c r="E81" s="272"/>
-      <c r="F81" s="83"/>
-      <c r="G81" s="84"/>
-      <c r="H81" s="84"/>
-      <c r="I81" s="85"/>
-      <c r="J81" s="85"/>
-      <c r="K81" s="85"/>
-      <c r="L81" s="86"/>
-      <c r="M81" s="206"/>
-      <c r="N81" s="207"/>
-    </row>
-    <row r="82" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M82" s="17"/>
-      <c r="N82" s="17"/>
+      <c r="D86" s="82"/>
+      <c r="E86" s="204"/>
+      <c r="F86" s="83"/>
+      <c r="G86" s="84"/>
+      <c r="H86" s="84"/>
+      <c r="I86" s="85"/>
+      <c r="J86" s="85"/>
+      <c r="K86" s="85"/>
+      <c r="L86" s="86"/>
+      <c r="M86" s="265"/>
+      <c r="N86" s="266"/>
+    </row>
+    <row r="87" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="M57:N57"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="M55:N55"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M65:N65"/>
+    <mergeCell ref="M66:N66"/>
+    <mergeCell ref="M67:N67"/>
+    <mergeCell ref="M68:N68"/>
+    <mergeCell ref="M69:N69"/>
+    <mergeCell ref="M70:N70"/>
+    <mergeCell ref="M80:N80"/>
+    <mergeCell ref="M81:N81"/>
+    <mergeCell ref="M71:N71"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="A5:A38"/>
+    <mergeCell ref="D2:D3"/>
     <mergeCell ref="M2:N3"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="M11:N11"/>
@@ -6286,38 +6607,28 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="M7:N7"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="B11:B42"/>
-    <mergeCell ref="A5:A42"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B43:B49"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="A50:A81"/>
-    <mergeCell ref="B50:B81"/>
-    <mergeCell ref="A43:A49"/>
-    <mergeCell ref="M81:N81"/>
-    <mergeCell ref="M59:N59"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="M61:N61"/>
     <mergeCell ref="M62:N62"/>
     <mergeCell ref="M63:N63"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M65:N65"/>
-    <mergeCell ref="M75:N75"/>
-    <mergeCell ref="M76:N76"/>
-    <mergeCell ref="M66:N66"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="B11:B38"/>
+    <mergeCell ref="B39:B54"/>
+    <mergeCell ref="A39:A54"/>
+    <mergeCell ref="B55:B86"/>
+    <mergeCell ref="A55:A86"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="29" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="28" orientation="landscape" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0">
     <oddHeader>&amp;C&amp;F</oddHeader>
     <oddFooter>&amp;R&amp;D</oddFooter>
@@ -6332,7 +6643,7 @@
   </sheetPr>
   <dimension ref="A1:CU22"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -7845,7 +8156,7 @@
       <c r="L1" s="126"/>
     </row>
     <row r="2" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="259" t="s">
+      <c r="A2" s="275" t="s">
         <v>179</v>
       </c>
       <c r="B2" s="146">
@@ -7881,7 +8192,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="260"/>
+      <c r="A3" s="276"/>
       <c r="B3" s="133">
         <v>2</v>
       </c>
@@ -7905,7 +8216,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="260"/>
+      <c r="A4" s="276"/>
       <c r="B4" s="175">
         <v>3</v>
       </c>
@@ -7939,7 +8250,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="260"/>
+      <c r="A5" s="276"/>
       <c r="B5" s="146">
         <v>4</v>
       </c>
@@ -7973,7 +8284,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="260"/>
+      <c r="A6" s="276"/>
       <c r="B6" s="133">
         <v>5</v>
       </c>
@@ -7997,7 +8308,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="261"/>
+      <c r="A7" s="277"/>
       <c r="B7" s="146">
         <v>6</v>
       </c>
@@ -8045,7 +8356,7 @@
       <c r="L8" s="152"/>
     </row>
     <row r="9" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="259" t="s">
+      <c r="A9" s="275" t="s">
         <v>180</v>
       </c>
       <c r="B9" s="146">
@@ -8081,7 +8392,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="261"/>
+      <c r="A10" s="277"/>
       <c r="B10" s="146">
         <v>2</v>
       </c>
@@ -8126,4 +8437,16 @@
     <oddFooter>&amp;R&amp;D</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated documentation - new signals for polarity switch motors.
</commit_message>
<xml_diff>
--- a/doc/truth_table_safety_plc.xlsx
+++ b/doc/truth_table_safety_plc.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="TRUE TABLE" sheetId="7" r:id="rId1"/>
+    <sheet name="TRUTH TABLE" sheetId="7" r:id="rId1"/>
     <sheet name="EE" sheetId="9" r:id="rId2"/>
     <sheet name="PC" sheetId="10" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="11" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'TRUE TABLE'!$A$1:$Q$83</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'TRUTH TABLE'!$A$1:$Q$83</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="395">
   <si>
     <t>NA</t>
   </si>
@@ -1693,6 +1693,78 @@
       </rPr>
       <t>: PC off</t>
     </r>
+  </si>
+  <si>
+    <t>$(P):PolSw-1:cmdMove</t>
+  </si>
+  <si>
+    <t>POLSW_1_MTR_ON</t>
+  </si>
+  <si>
+    <t>POLSW_2_MTR_ON</t>
+  </si>
+  <si>
+    <t>$(P):PolSw-2:cmdMove</t>
+  </si>
+  <si>
+    <t>$(P):PolSw:dirPos1</t>
+  </si>
+  <si>
+    <t>$(P):PolSw:dirPos2</t>
+  </si>
+  <si>
+    <t>POLSW_DIR_POS1</t>
+  </si>
+  <si>
+    <t>POLSW_DIR_POS2</t>
+  </si>
+  <si>
+    <t>Motor 1 power on</t>
+  </si>
+  <si>
+    <t>Motor 2 power on</t>
+  </si>
+  <si>
+    <t>Direction towards pos1 switch</t>
+  </si>
+  <si>
+    <t>Direction towards pos2 switch</t>
+  </si>
+  <si>
+    <t>Q0.5</t>
+  </si>
+  <si>
+    <t>Q2.5</t>
+  </si>
+  <si>
+    <t>Q3.0</t>
+  </si>
+  <si>
+    <t>Q3.1</t>
+  </si>
+  <si>
+    <t>When logical 1 motor moves towards pos1 switch (I1.2 for motor 1, I3.2 for motor 2)</t>
+  </si>
+  <si>
+    <t>When logical 1 motor moves toeards pos2 switch (I1.3 for motor 1, I3.3 for motor 2)</t>
+  </si>
+  <si>
+    <t>When logical 1 powers  motor 1</t>
+  </si>
+  <si>
+    <t>When logical 1 powers motor 2</t>
+  </si>
+  <si>
+    <t>1 when switching  polarity  until (GERSEMI_POLSW_1_POS1 =  1 AND POLSW_DIR_POS1 = 1) OR (GERSEMI_POLSW_1_POS2 =  1 AND POLSW_DIR_POS2 = 1)</t>
+  </si>
+  <si>
+    <t>1 when switching  polarity  until (GERSEMI_POLSW_2_POS1 =  1 AND POLSW_DIR_POS1 = 1) OR (GERSEMI_POLSW_2_POS2 =  1 AND POLSW_DIR_POS2 = 1)</t>
+  </si>
+  <si>
+    <t>1 when requested polarity switch towards pos1</t>
+  </si>
+  <si>
+    <t>1 when requested polarity switch towards pos2</t>
   </si>
 </sst>
 </file>
@@ -2663,7 +2735,7 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="275">
+  <cellXfs count="276">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -3307,6 +3379,213 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3322,213 +3601,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -3537,6 +3609,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="42" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3936,11 +4011,11 @@
   </sheetPr>
   <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="25" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="25" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="K47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="C73" sqref="A73:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3983,67 +4058,67 @@
       <c r="N1" s="86"/>
     </row>
     <row r="2" spans="1:22" s="87" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="226" t="s">
+      <c r="A2" s="245" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="229"/>
-      <c r="C2" s="230"/>
-      <c r="D2" s="220" t="s">
+      <c r="B2" s="248"/>
+      <c r="C2" s="249"/>
+      <c r="D2" s="255" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="208" t="s">
+      <c r="E2" s="270" t="s">
         <v>246</v>
       </c>
-      <c r="F2" s="220" t="s">
+      <c r="F2" s="255" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="224" t="s">
+      <c r="G2" s="261" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="225"/>
-      <c r="I2" s="222" t="s">
+      <c r="H2" s="262"/>
+      <c r="I2" s="259" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="222"/>
-      <c r="K2" s="220" t="s">
+      <c r="J2" s="259"/>
+      <c r="K2" s="255" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="218" t="s">
+      <c r="L2" s="257" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="239" t="s">
+      <c r="M2" s="231" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="240"/>
+      <c r="N2" s="232"/>
       <c r="O2" s="88"/>
       <c r="P2" s="88"/>
       <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:22" s="87" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="227"/>
-      <c r="B3" s="231"/>
-      <c r="C3" s="232"/>
-      <c r="D3" s="221"/>
-      <c r="E3" s="209"/>
-      <c r="F3" s="221"/>
+      <c r="A3" s="246"/>
+      <c r="B3" s="250"/>
+      <c r="C3" s="251"/>
+      <c r="D3" s="256"/>
+      <c r="E3" s="271"/>
+      <c r="F3" s="256"/>
       <c r="G3" s="193" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="193" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="223"/>
-      <c r="J3" s="223"/>
-      <c r="K3" s="223"/>
-      <c r="L3" s="219"/>
-      <c r="M3" s="241"/>
-      <c r="N3" s="242"/>
+      <c r="I3" s="260"/>
+      <c r="J3" s="260"/>
+      <c r="K3" s="260"/>
+      <c r="L3" s="258"/>
+      <c r="M3" s="233"/>
+      <c r="N3" s="234"/>
       <c r="O3" s="88"/>
       <c r="P3" s="88"/>
       <c r="Q3" s="88"/>
     </row>
     <row r="4" spans="1:22" s="97" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="228"/>
+      <c r="A4" s="247"/>
       <c r="B4" s="89" t="s">
         <v>14</v>
       </c>
@@ -4069,19 +4144,19 @@
       <c r="L4" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="243" t="s">
+      <c r="M4" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="N4" s="244"/>
+      <c r="N4" s="236"/>
       <c r="O4" s="96"/>
       <c r="P4" s="96"/>
       <c r="Q4" s="96"/>
     </row>
     <row r="5" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="236" t="s">
+      <c r="A5" s="216" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="233" t="s">
+      <c r="B5" s="252" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="98">
@@ -4106,17 +4181,17 @@
       <c r="L5" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="251" t="s">
+      <c r="M5" s="243" t="s">
         <v>202</v>
       </c>
-      <c r="N5" s="252"/>
+      <c r="N5" s="244"/>
       <c r="O5" s="104"/>
       <c r="P5" s="104"/>
       <c r="Q5" s="104"/>
     </row>
     <row r="6" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="237"/>
-      <c r="B6" s="234"/>
+      <c r="A6" s="217"/>
+      <c r="B6" s="253"/>
       <c r="C6" s="106">
         <v>2</v>
       </c>
@@ -4139,17 +4214,17 @@
       <c r="L6" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="249" t="s">
+      <c r="M6" s="241" t="s">
         <v>202</v>
       </c>
-      <c r="N6" s="250"/>
+      <c r="N6" s="242"/>
       <c r="O6" s="104"/>
       <c r="P6" s="104"/>
       <c r="Q6" s="104"/>
     </row>
     <row r="7" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="237"/>
-      <c r="B7" s="234"/>
+      <c r="A7" s="217"/>
+      <c r="B7" s="253"/>
       <c r="C7" s="106">
         <v>3</v>
       </c>
@@ -4172,17 +4247,17 @@
       <c r="L7" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="249" t="s">
+      <c r="M7" s="241" t="s">
         <v>294</v>
       </c>
-      <c r="N7" s="250"/>
+      <c r="N7" s="242"/>
       <c r="O7" s="104"/>
       <c r="P7" s="104"/>
       <c r="Q7" s="104"/>
     </row>
     <row r="8" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="237"/>
-      <c r="B8" s="234"/>
+      <c r="A8" s="217"/>
+      <c r="B8" s="253"/>
       <c r="C8" s="106">
         <v>4</v>
       </c>
@@ -4205,17 +4280,17 @@
       <c r="L8" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="249" t="s">
+      <c r="M8" s="241" t="s">
         <v>295</v>
       </c>
-      <c r="N8" s="250"/>
+      <c r="N8" s="242"/>
       <c r="O8" s="104"/>
       <c r="P8" s="104"/>
       <c r="Q8" s="104"/>
     </row>
     <row r="9" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="237"/>
-      <c r="B9" s="234"/>
+      <c r="A9" s="217"/>
+      <c r="B9" s="253"/>
       <c r="C9" s="106">
         <v>5</v>
       </c>
@@ -4238,17 +4313,17 @@
       <c r="L9" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="249" t="s">
+      <c r="M9" s="241" t="s">
         <v>296</v>
       </c>
-      <c r="N9" s="250"/>
+      <c r="N9" s="242"/>
       <c r="O9" s="104"/>
       <c r="P9" s="104"/>
       <c r="Q9" s="104"/>
     </row>
     <row r="10" spans="1:22" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="237"/>
-      <c r="B10" s="235"/>
+      <c r="A10" s="217"/>
+      <c r="B10" s="254"/>
       <c r="C10" s="113">
         <v>6</v>
       </c>
@@ -4271,17 +4346,17 @@
       <c r="L10" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="249" t="s">
+      <c r="M10" s="241" t="s">
         <v>297</v>
       </c>
-      <c r="N10" s="250"/>
+      <c r="N10" s="242"/>
       <c r="O10" s="104"/>
       <c r="P10" s="104"/>
       <c r="Q10" s="104"/>
     </row>
     <row r="11" spans="1:22" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="237"/>
-      <c r="B11" s="263" t="s">
+      <c r="A11" s="217"/>
+      <c r="B11" s="213" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="119">
@@ -4312,17 +4387,17 @@
       <c r="L11" s="124">
         <v>1</v>
       </c>
-      <c r="M11" s="245" t="s">
+      <c r="M11" s="237" t="s">
         <v>85</v>
       </c>
-      <c r="N11" s="246"/>
+      <c r="N11" s="238"/>
       <c r="O11" s="104"/>
       <c r="P11" s="104"/>
       <c r="Q11" s="104"/>
     </row>
     <row r="12" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="237"/>
-      <c r="B12" s="264"/>
+      <c r="A12" s="217"/>
+      <c r="B12" s="214"/>
       <c r="C12" s="125">
         <v>2</v>
       </c>
@@ -4351,15 +4426,15 @@
       <c r="L12" s="130">
         <v>1</v>
       </c>
-      <c r="M12" s="247"/>
-      <c r="N12" s="248"/>
+      <c r="M12" s="239"/>
+      <c r="N12" s="240"/>
       <c r="O12" s="104"/>
       <c r="P12" s="104"/>
       <c r="Q12" s="104"/>
     </row>
     <row r="13" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="237"/>
-      <c r="B13" s="264"/>
+      <c r="A13" s="217"/>
+      <c r="B13" s="214"/>
       <c r="C13" s="131">
         <v>3</v>
       </c>
@@ -4399,8 +4474,8 @@
       <c r="Q13" s="104"/>
     </row>
     <row r="14" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="237"/>
-      <c r="B14" s="264"/>
+      <c r="A14" s="217"/>
+      <c r="B14" s="214"/>
       <c r="C14" s="125">
         <v>4</v>
       </c>
@@ -4445,8 +4520,8 @@
       <c r="V14" s="137"/>
     </row>
     <row r="15" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="237"/>
-      <c r="B15" s="264"/>
+      <c r="A15" s="217"/>
+      <c r="B15" s="214"/>
       <c r="C15" s="131">
         <v>5</v>
       </c>
@@ -4491,8 +4566,8 @@
       <c r="V15" s="137"/>
     </row>
     <row r="16" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="237"/>
-      <c r="B16" s="264"/>
+      <c r="A16" s="217"/>
+      <c r="B16" s="214"/>
       <c r="C16" s="125">
         <v>6</v>
       </c>
@@ -4535,8 +4610,8 @@
       <c r="V16" s="137"/>
     </row>
     <row r="17" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="237"/>
-      <c r="B17" s="264"/>
+      <c r="A17" s="217"/>
+      <c r="B17" s="214"/>
       <c r="C17" s="131">
         <v>7</v>
       </c>
@@ -4581,8 +4656,8 @@
       <c r="V17" s="137"/>
     </row>
     <row r="18" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="237"/>
-      <c r="B18" s="264"/>
+      <c r="A18" s="217"/>
+      <c r="B18" s="214"/>
       <c r="C18" s="125">
         <v>8</v>
       </c>
@@ -4627,8 +4702,8 @@
       <c r="V18" s="137"/>
     </row>
     <row r="19" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="237"/>
-      <c r="B19" s="264"/>
+      <c r="A19" s="217"/>
+      <c r="B19" s="214"/>
       <c r="C19" s="131">
         <v>9</v>
       </c>
@@ -4673,8 +4748,8 @@
       <c r="V19" s="137"/>
     </row>
     <row r="20" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="237"/>
-      <c r="B20" s="264"/>
+      <c r="A20" s="217"/>
+      <c r="B20" s="214"/>
       <c r="C20" s="125">
         <v>10</v>
       </c>
@@ -4714,8 +4789,8 @@
       <c r="Q20" s="104"/>
     </row>
     <row r="21" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="237"/>
-      <c r="B21" s="264"/>
+      <c r="A21" s="217"/>
+      <c r="B21" s="214"/>
       <c r="C21" s="131">
         <v>11</v>
       </c>
@@ -4755,8 +4830,8 @@
       <c r="Q21" s="104"/>
     </row>
     <row r="22" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="237"/>
-      <c r="B22" s="264"/>
+      <c r="A22" s="217"/>
+      <c r="B22" s="214"/>
       <c r="C22" s="125">
         <v>12</v>
       </c>
@@ -4794,8 +4869,8 @@
       <c r="Q22" s="104"/>
     </row>
     <row r="23" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="237"/>
-      <c r="B23" s="264"/>
+      <c r="A23" s="217"/>
+      <c r="B23" s="214"/>
       <c r="C23" s="131">
         <v>13</v>
       </c>
@@ -4835,8 +4910,8 @@
       <c r="Q23" s="104"/>
     </row>
     <row r="24" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="237"/>
-      <c r="B24" s="264"/>
+      <c r="A24" s="217"/>
+      <c r="B24" s="214"/>
       <c r="C24" s="125">
         <v>14</v>
       </c>
@@ -4876,8 +4951,8 @@
       <c r="Q24" s="104"/>
     </row>
     <row r="25" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="237"/>
-      <c r="B25" s="264"/>
+      <c r="A25" s="217"/>
+      <c r="B25" s="214"/>
       <c r="C25" s="131">
         <v>15</v>
       </c>
@@ -4906,17 +4981,17 @@
       <c r="L25" s="130">
         <v>1</v>
       </c>
-      <c r="M25" s="255" t="s">
+      <c r="M25" s="211" t="s">
         <v>359</v>
       </c>
-      <c r="N25" s="256"/>
+      <c r="N25" s="212"/>
       <c r="O25" s="104"/>
       <c r="P25" s="104"/>
       <c r="Q25" s="104"/>
     </row>
     <row r="26" spans="1:22" s="141" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="237"/>
-      <c r="B26" s="264"/>
+      <c r="A26" s="217"/>
+      <c r="B26" s="214"/>
       <c r="C26" s="131">
         <v>16</v>
       </c>
@@ -4945,17 +5020,17 @@
       <c r="L26" s="130">
         <v>1</v>
       </c>
-      <c r="M26" s="255" t="s">
+      <c r="M26" s="211" t="s">
         <v>46</v>
       </c>
-      <c r="N26" s="256"/>
+      <c r="N26" s="212"/>
       <c r="O26" s="140"/>
       <c r="P26" s="140"/>
       <c r="Q26" s="140"/>
     </row>
     <row r="27" spans="1:22" s="143" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="237"/>
-      <c r="B27" s="264"/>
+      <c r="A27" s="217"/>
+      <c r="B27" s="214"/>
       <c r="C27" s="125">
         <v>17</v>
       </c>
@@ -4984,17 +5059,17 @@
       <c r="L27" s="130">
         <v>1</v>
       </c>
-      <c r="M27" s="255" t="s">
+      <c r="M27" s="211" t="s">
         <v>360</v>
       </c>
-      <c r="N27" s="256"/>
+      <c r="N27" s="212"/>
       <c r="O27" s="142"/>
       <c r="P27" s="142"/>
       <c r="Q27" s="142"/>
     </row>
     <row r="28" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="237"/>
-      <c r="B28" s="264"/>
+      <c r="A28" s="217"/>
+      <c r="B28" s="214"/>
       <c r="C28" s="131">
         <v>18</v>
       </c>
@@ -5023,17 +5098,17 @@
       <c r="L28" s="130">
         <v>1</v>
       </c>
-      <c r="M28" s="255" t="s">
+      <c r="M28" s="211" t="s">
         <v>359</v>
       </c>
-      <c r="N28" s="256"/>
+      <c r="N28" s="212"/>
       <c r="O28" s="104"/>
       <c r="P28" s="104"/>
       <c r="Q28" s="104"/>
     </row>
     <row r="29" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="237"/>
-      <c r="B29" s="264"/>
+      <c r="A29" s="217"/>
+      <c r="B29" s="214"/>
       <c r="C29" s="131">
         <v>19</v>
       </c>
@@ -5062,17 +5137,17 @@
       <c r="L29" s="130">
         <v>1</v>
       </c>
-      <c r="M29" s="255" t="s">
+      <c r="M29" s="211" t="s">
         <v>46</v>
       </c>
-      <c r="N29" s="256"/>
+      <c r="N29" s="212"/>
       <c r="O29" s="104"/>
       <c r="P29" s="104"/>
       <c r="Q29" s="104"/>
     </row>
     <row r="30" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="237"/>
-      <c r="B30" s="264"/>
+      <c r="A30" s="217"/>
+      <c r="B30" s="214"/>
       <c r="C30" s="125">
         <v>20</v>
       </c>
@@ -5101,17 +5176,17 @@
       <c r="L30" s="130">
         <v>1</v>
       </c>
-      <c r="M30" s="255" t="s">
+      <c r="M30" s="211" t="s">
         <v>360</v>
       </c>
-      <c r="N30" s="256"/>
+      <c r="N30" s="212"/>
       <c r="O30" s="104"/>
       <c r="P30" s="104"/>
       <c r="Q30" s="104"/>
     </row>
     <row r="31" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="237"/>
-      <c r="B31" s="264"/>
+      <c r="A31" s="217"/>
+      <c r="B31" s="214"/>
       <c r="C31" s="131">
         <v>21</v>
       </c>
@@ -5147,8 +5222,8 @@
       <c r="Q31" s="104"/>
     </row>
     <row r="32" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="237"/>
-      <c r="B32" s="264"/>
+      <c r="A32" s="217"/>
+      <c r="B32" s="214"/>
       <c r="C32" s="131">
         <v>22</v>
       </c>
@@ -5186,8 +5261,8 @@
       <c r="Q32" s="104"/>
     </row>
     <row r="33" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="237"/>
-      <c r="B33" s="264"/>
+      <c r="A33" s="217"/>
+      <c r="B33" s="214"/>
       <c r="C33" s="131">
         <v>23</v>
       </c>
@@ -5225,8 +5300,8 @@
       <c r="Q33" s="104"/>
     </row>
     <row r="34" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="237"/>
-      <c r="B34" s="264"/>
+      <c r="A34" s="217"/>
+      <c r="B34" s="214"/>
       <c r="C34" s="131">
         <v>24</v>
       </c>
@@ -5264,8 +5339,8 @@
       <c r="Q34" s="104"/>
     </row>
     <row r="35" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="237"/>
-      <c r="B35" s="264"/>
+      <c r="A35" s="217"/>
+      <c r="B35" s="214"/>
       <c r="C35" s="131">
         <v>25</v>
       </c>
@@ -5297,8 +5372,8 @@
       <c r="Q35" s="104"/>
     </row>
     <row r="36" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="237"/>
-      <c r="B36" s="264"/>
+      <c r="A36" s="217"/>
+      <c r="B36" s="214"/>
       <c r="C36" s="131">
         <v>26</v>
       </c>
@@ -5330,8 +5405,8 @@
       <c r="Q36" s="104"/>
     </row>
     <row r="37" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="237"/>
-      <c r="B37" s="264"/>
+      <c r="A37" s="217"/>
+      <c r="B37" s="214"/>
       <c r="C37" s="131">
         <v>27</v>
       </c>
@@ -5363,8 +5438,8 @@
       <c r="Q37" s="104"/>
     </row>
     <row r="38" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="237"/>
-      <c r="B38" s="264"/>
+      <c r="A38" s="217"/>
+      <c r="B38" s="214"/>
       <c r="C38" s="131">
         <v>28</v>
       </c>
@@ -5396,8 +5471,8 @@
       <c r="Q38" s="104"/>
     </row>
     <row r="39" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="237"/>
-      <c r="B39" s="264"/>
+      <c r="A39" s="217"/>
+      <c r="B39" s="214"/>
       <c r="C39" s="131">
         <v>29</v>
       </c>
@@ -5429,8 +5504,8 @@
       <c r="Q39" s="104"/>
     </row>
     <row r="40" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="237"/>
-      <c r="B40" s="264"/>
+      <c r="A40" s="217"/>
+      <c r="B40" s="214"/>
       <c r="C40" s="131">
         <v>30</v>
       </c>
@@ -5462,8 +5537,8 @@
       <c r="Q40" s="104"/>
     </row>
     <row r="41" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="237"/>
-      <c r="B41" s="264"/>
+      <c r="A41" s="217"/>
+      <c r="B41" s="214"/>
       <c r="C41" s="131">
         <v>31</v>
       </c>
@@ -5476,15 +5551,15 @@
       <c r="J41" s="129"/>
       <c r="K41" s="129"/>
       <c r="L41" s="146"/>
-      <c r="M41" s="255"/>
-      <c r="N41" s="256"/>
+      <c r="M41" s="211"/>
+      <c r="N41" s="212"/>
       <c r="O41" s="104"/>
       <c r="P41" s="104"/>
       <c r="Q41" s="104"/>
     </row>
     <row r="42" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="238"/>
-      <c r="B42" s="265"/>
+      <c r="A42" s="218"/>
+      <c r="B42" s="215"/>
       <c r="C42" s="147">
         <v>32</v>
       </c>
@@ -5497,15 +5572,15 @@
       <c r="J42" s="150"/>
       <c r="K42" s="150"/>
       <c r="L42" s="151"/>
-      <c r="M42" s="253"/>
-      <c r="N42" s="254"/>
+      <c r="M42" s="229"/>
+      <c r="N42" s="230"/>
       <c r="O42" s="104"/>
       <c r="P42" s="104"/>
       <c r="Q42" s="104"/>
     </row>
     <row r="43" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="236"/>
-      <c r="B43" s="263" t="s">
+      <c r="A43" s="216"/>
+      <c r="B43" s="213" t="s">
         <v>83</v>
       </c>
       <c r="C43" s="119">
@@ -5532,15 +5607,15 @@
       <c r="L43" s="152" t="s">
         <v>177</v>
       </c>
-      <c r="M43" s="261"/>
-      <c r="N43" s="262"/>
+      <c r="M43" s="209"/>
+      <c r="N43" s="210"/>
       <c r="O43" s="104"/>
       <c r="P43" s="104"/>
       <c r="Q43" s="104"/>
     </row>
     <row r="44" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="237"/>
-      <c r="B44" s="264"/>
+      <c r="A44" s="217"/>
+      <c r="B44" s="214"/>
       <c r="C44" s="131">
         <v>2</v>
       </c>
@@ -5572,8 +5647,8 @@
       <c r="Q44" s="104"/>
     </row>
     <row r="45" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="237"/>
-      <c r="B45" s="264"/>
+      <c r="A45" s="217"/>
+      <c r="B45" s="214"/>
       <c r="C45" s="155">
         <v>3</v>
       </c>
@@ -5598,17 +5673,17 @@
       <c r="L45" s="152">
         <v>1</v>
       </c>
-      <c r="M45" s="255" t="s">
+      <c r="M45" s="211" t="s">
         <v>179</v>
       </c>
-      <c r="N45" s="256"/>
+      <c r="N45" s="212"/>
       <c r="O45" s="104"/>
       <c r="P45" s="104"/>
       <c r="Q45" s="104"/>
     </row>
     <row r="46" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="237"/>
-      <c r="B46" s="264"/>
+      <c r="A46" s="217"/>
+      <c r="B46" s="214"/>
       <c r="C46" s="125">
         <v>4</v>
       </c>
@@ -5642,8 +5717,8 @@
       <c r="Q46" s="104"/>
     </row>
     <row r="47" spans="1:17" s="143" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="237"/>
-      <c r="B47" s="264"/>
+      <c r="A47" s="217"/>
+      <c r="B47" s="214"/>
       <c r="C47" s="125">
         <v>5</v>
       </c>
@@ -5677,8 +5752,8 @@
       <c r="Q47" s="142"/>
     </row>
     <row r="48" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="237"/>
-      <c r="B48" s="264"/>
+      <c r="A48" s="217"/>
+      <c r="B48" s="214"/>
       <c r="C48" s="125">
         <v>6</v>
       </c>
@@ -5712,8 +5787,8 @@
       <c r="Q48" s="104"/>
     </row>
     <row r="49" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="237"/>
-      <c r="B49" s="264"/>
+      <c r="A49" s="217"/>
+      <c r="B49" s="214"/>
       <c r="C49" s="125">
         <v>7</v>
       </c>
@@ -5747,8 +5822,8 @@
       <c r="Q49" s="104"/>
     </row>
     <row r="50" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="237"/>
-      <c r="B50" s="264"/>
+      <c r="A50" s="217"/>
+      <c r="B50" s="214"/>
       <c r="C50" s="125">
         <v>8</v>
       </c>
@@ -5780,8 +5855,8 @@
       <c r="Q50" s="104"/>
     </row>
     <row r="51" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="237"/>
-      <c r="B51" s="264"/>
+      <c r="A51" s="217"/>
+      <c r="B51" s="214"/>
       <c r="C51" s="125">
         <v>9</v>
       </c>
@@ -5813,8 +5888,8 @@
       <c r="Q51" s="104"/>
     </row>
     <row r="52" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="237"/>
-      <c r="B52" s="264"/>
+      <c r="A52" s="217"/>
+      <c r="B52" s="214"/>
       <c r="C52" s="125">
         <v>10</v>
       </c>
@@ -5846,8 +5921,8 @@
       <c r="Q52" s="104"/>
     </row>
     <row r="53" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="237"/>
-      <c r="B53" s="264"/>
+      <c r="A53" s="217"/>
+      <c r="B53" s="214"/>
       <c r="C53" s="125">
         <v>11</v>
       </c>
@@ -5879,8 +5954,8 @@
       <c r="Q53" s="104"/>
     </row>
     <row r="54" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="237"/>
-      <c r="B54" s="264"/>
+      <c r="A54" s="217"/>
+      <c r="B54" s="214"/>
       <c r="C54" s="125">
         <v>12</v>
       </c>
@@ -5900,8 +5975,8 @@
       <c r="Q54" s="104"/>
     </row>
     <row r="55" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="237"/>
-      <c r="B55" s="264"/>
+      <c r="A55" s="217"/>
+      <c r="B55" s="214"/>
       <c r="C55" s="125">
         <v>13</v>
       </c>
@@ -5921,8 +5996,8 @@
       <c r="Q55" s="104"/>
     </row>
     <row r="56" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="237"/>
-      <c r="B56" s="264"/>
+      <c r="A56" s="217"/>
+      <c r="B56" s="214"/>
       <c r="C56" s="125">
         <v>14</v>
       </c>
@@ -5942,8 +6017,8 @@
       <c r="Q56" s="104"/>
     </row>
     <row r="57" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="237"/>
-      <c r="B57" s="264"/>
+      <c r="A57" s="217"/>
+      <c r="B57" s="214"/>
       <c r="C57" s="125">
         <v>15</v>
       </c>
@@ -5963,8 +6038,8 @@
       <c r="Q57" s="104"/>
     </row>
     <row r="58" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="238"/>
-      <c r="B58" s="265"/>
+      <c r="A58" s="218"/>
+      <c r="B58" s="215"/>
       <c r="C58" s="125">
         <v>16</v>
       </c>
@@ -5984,10 +6059,10 @@
       <c r="Q58" s="104"/>
     </row>
     <row r="59" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="259" t="s">
+      <c r="A59" s="207" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="257" t="s">
+      <c r="B59" s="205" t="s">
         <v>55</v>
       </c>
       <c r="C59" s="156">
@@ -6018,15 +6093,15 @@
       <c r="L59" s="200" t="s">
         <v>236</v>
       </c>
-      <c r="M59" s="266"/>
-      <c r="N59" s="267"/>
+      <c r="M59" s="219"/>
+      <c r="N59" s="220"/>
       <c r="O59" s="104"/>
       <c r="P59" s="104"/>
       <c r="Q59" s="104"/>
     </row>
     <row r="60" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="260"/>
-      <c r="B60" s="258"/>
+      <c r="A60" s="208"/>
+      <c r="B60" s="206"/>
       <c r="C60" s="161">
         <v>2</v>
       </c>
@@ -6064,8 +6139,8 @@
       <c r="Q60" s="104"/>
     </row>
     <row r="61" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="260"/>
-      <c r="B61" s="258"/>
+      <c r="A61" s="208"/>
+      <c r="B61" s="206"/>
       <c r="C61" s="156">
         <v>3</v>
       </c>
@@ -6105,8 +6180,8 @@
       <c r="Q61" s="104"/>
     </row>
     <row r="62" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="260"/>
-      <c r="B62" s="258"/>
+      <c r="A62" s="208"/>
+      <c r="B62" s="206"/>
       <c r="C62" s="161">
         <v>4</v>
       </c>
@@ -6146,8 +6221,8 @@
       <c r="Q62" s="104"/>
     </row>
     <row r="63" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="260"/>
-      <c r="B63" s="258"/>
+      <c r="A63" s="208"/>
+      <c r="B63" s="206"/>
       <c r="C63" s="156">
         <v>5</v>
       </c>
@@ -6185,8 +6260,8 @@
       <c r="Q63" s="170"/>
     </row>
     <row r="64" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="260"/>
-      <c r="B64" s="258"/>
+      <c r="A64" s="208"/>
+      <c r="B64" s="206"/>
       <c r="C64" s="161">
         <v>6</v>
       </c>
@@ -6226,8 +6301,8 @@
       <c r="Q64" s="170"/>
     </row>
     <row r="65" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="260"/>
-      <c r="B65" s="258"/>
+      <c r="A65" s="208"/>
+      <c r="B65" s="206"/>
       <c r="C65" s="156">
         <v>7</v>
       </c>
@@ -6267,8 +6342,8 @@
       <c r="Q65" s="170"/>
     </row>
     <row r="66" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="260"/>
-      <c r="B66" s="258"/>
+      <c r="A66" s="208"/>
+      <c r="B66" s="206"/>
       <c r="C66" s="161">
         <v>8</v>
       </c>
@@ -6297,17 +6372,17 @@
       <c r="L66" s="204" t="s">
         <v>181</v>
       </c>
-      <c r="M66" s="216" t="s">
+      <c r="M66" s="265" t="s">
         <v>47</v>
       </c>
-      <c r="N66" s="217"/>
+      <c r="N66" s="266"/>
       <c r="O66" s="170"/>
       <c r="P66" s="170"/>
       <c r="Q66" s="170"/>
     </row>
     <row r="67" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="260"/>
-      <c r="B67" s="258"/>
+      <c r="A67" s="208"/>
+      <c r="B67" s="206"/>
       <c r="C67" s="156">
         <v>9</v>
       </c>
@@ -6336,17 +6411,17 @@
       <c r="L67" s="204" t="s">
         <v>181</v>
       </c>
-      <c r="M67" s="216" t="s">
+      <c r="M67" s="265" t="s">
         <v>47</v>
       </c>
-      <c r="N67" s="217"/>
+      <c r="N67" s="266"/>
       <c r="O67" s="170"/>
       <c r="P67" s="170"/>
       <c r="Q67" s="170"/>
     </row>
     <row r="68" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="260"/>
-      <c r="B68" s="258"/>
+      <c r="A68" s="208"/>
+      <c r="B68" s="206"/>
       <c r="C68" s="161">
         <v>10</v>
       </c>
@@ -6375,17 +6450,17 @@
       <c r="L68" s="203" t="s">
         <v>180</v>
       </c>
-      <c r="M68" s="270" t="s">
+      <c r="M68" s="223" t="s">
         <v>367</v>
       </c>
-      <c r="N68" s="271"/>
+      <c r="N68" s="224"/>
       <c r="O68" s="170"/>
       <c r="P68" s="170"/>
       <c r="Q68" s="170"/>
     </row>
     <row r="69" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="260"/>
-      <c r="B69" s="258"/>
+      <c r="A69" s="208"/>
+      <c r="B69" s="206"/>
       <c r="C69" s="156">
         <v>11</v>
       </c>
@@ -6414,17 +6489,17 @@
       <c r="L69" s="203" t="s">
         <v>180</v>
       </c>
-      <c r="M69" s="270" t="s">
+      <c r="M69" s="223" t="s">
         <v>367</v>
       </c>
-      <c r="N69" s="271"/>
+      <c r="N69" s="224"/>
       <c r="O69" s="170"/>
       <c r="P69" s="170"/>
       <c r="Q69" s="170"/>
     </row>
     <row r="70" spans="1:17" s="171" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="260"/>
-      <c r="B70" s="258"/>
+      <c r="A70" s="208"/>
+      <c r="B70" s="206"/>
       <c r="C70" s="161">
         <v>12</v>
       </c>
@@ -6453,15 +6528,15 @@
       <c r="L70" s="203" t="s">
         <v>304</v>
       </c>
-      <c r="M70" s="210"/>
-      <c r="N70" s="211"/>
+      <c r="M70" s="225"/>
+      <c r="N70" s="226"/>
       <c r="O70" s="170"/>
       <c r="P70" s="170"/>
       <c r="Q70" s="170"/>
     </row>
     <row r="71" spans="1:17" s="171" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="260"/>
-      <c r="B71" s="258"/>
+      <c r="A71" s="208"/>
+      <c r="B71" s="206"/>
       <c r="C71" s="156">
         <v>13</v>
       </c>
@@ -6490,15 +6565,15 @@
       <c r="L71" s="203" t="s">
         <v>304</v>
       </c>
-      <c r="M71" s="210"/>
-      <c r="N71" s="211"/>
+      <c r="M71" s="225"/>
+      <c r="N71" s="226"/>
       <c r="O71" s="170"/>
       <c r="P71" s="170"/>
       <c r="Q71" s="170"/>
     </row>
     <row r="72" spans="1:17" s="171" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="260"/>
-      <c r="B72" s="258"/>
+      <c r="A72" s="208"/>
+      <c r="B72" s="206"/>
       <c r="C72" s="161">
         <v>14</v>
       </c>
@@ -6527,99 +6602,163 @@
       <c r="L72" s="203" t="s">
         <v>304</v>
       </c>
-      <c r="M72" s="214"/>
-      <c r="N72" s="215"/>
+      <c r="M72" s="227"/>
+      <c r="N72" s="228"/>
       <c r="O72" s="170"/>
       <c r="P72" s="170"/>
       <c r="Q72" s="170"/>
     </row>
-    <row r="73" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="260"/>
-      <c r="B73" s="258"/>
+    <row r="73" spans="1:17" s="171" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="208"/>
+      <c r="B73" s="206"/>
       <c r="C73" s="156">
         <v>15</v>
       </c>
-      <c r="D73" s="162"/>
-      <c r="E73" s="163"/>
-      <c r="F73" s="164"/>
+      <c r="D73" s="162" t="s">
+        <v>372</v>
+      </c>
+      <c r="E73" s="163" t="s">
+        <v>371</v>
+      </c>
+      <c r="F73" s="164" t="s">
+        <v>379</v>
+      </c>
       <c r="G73" s="165"/>
-      <c r="H73" s="173"/>
-      <c r="I73" s="173"/>
-      <c r="J73" s="173"/>
+      <c r="H73" s="173" t="s">
+        <v>383</v>
+      </c>
+      <c r="I73" s="173" t="s">
+        <v>7</v>
+      </c>
+      <c r="J73" s="173" t="s">
+        <v>6</v>
+      </c>
       <c r="K73" s="173"/>
-      <c r="L73" s="174"/>
-      <c r="M73" s="210"/>
-      <c r="N73" s="211"/>
+      <c r="L73" s="174" t="s">
+        <v>391</v>
+      </c>
+      <c r="M73" s="223" t="s">
+        <v>389</v>
+      </c>
+      <c r="N73" s="224"/>
       <c r="O73" s="170"/>
       <c r="P73" s="170"/>
       <c r="Q73" s="170"/>
     </row>
-    <row r="74" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="260"/>
-      <c r="B74" s="258"/>
+    <row r="74" spans="1:17" s="171" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="208"/>
+      <c r="B74" s="206"/>
       <c r="C74" s="161">
         <v>16</v>
       </c>
-      <c r="D74" s="162"/>
-      <c r="E74" s="163"/>
-      <c r="F74" s="164"/>
+      <c r="D74" s="162" t="s">
+        <v>373</v>
+      </c>
+      <c r="E74" s="163" t="s">
+        <v>374</v>
+      </c>
+      <c r="F74" s="164" t="s">
+        <v>380</v>
+      </c>
       <c r="G74" s="165"/>
-      <c r="H74" s="165"/>
-      <c r="I74" s="173"/>
-      <c r="J74" s="173"/>
+      <c r="H74" s="165" t="s">
+        <v>384</v>
+      </c>
+      <c r="I74" s="173" t="s">
+        <v>7</v>
+      </c>
+      <c r="J74" s="173" t="s">
+        <v>6</v>
+      </c>
       <c r="K74" s="173"/>
-      <c r="L74" s="174"/>
-      <c r="M74" s="210"/>
-      <c r="N74" s="211"/>
+      <c r="L74" s="174" t="s">
+        <v>392</v>
+      </c>
+      <c r="M74" s="223" t="s">
+        <v>390</v>
+      </c>
+      <c r="N74" s="224"/>
       <c r="O74" s="170"/>
       <c r="P74" s="170"/>
       <c r="Q74" s="170"/>
     </row>
     <row r="75" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="260"/>
-      <c r="B75" s="258"/>
+      <c r="A75" s="208"/>
+      <c r="B75" s="206"/>
       <c r="C75" s="156">
         <v>17</v>
       </c>
-      <c r="D75" s="162"/>
-      <c r="E75" s="163"/>
-      <c r="F75" s="164"/>
+      <c r="D75" s="175" t="s">
+        <v>377</v>
+      </c>
+      <c r="E75" s="176" t="s">
+        <v>375</v>
+      </c>
+      <c r="F75" s="164" t="s">
+        <v>381</v>
+      </c>
       <c r="G75" s="165"/>
-      <c r="H75" s="165"/>
-      <c r="I75" s="173"/>
-      <c r="J75" s="173"/>
+      <c r="H75" s="165" t="s">
+        <v>385</v>
+      </c>
+      <c r="I75" s="173" t="s">
+        <v>7</v>
+      </c>
+      <c r="J75" s="173" t="s">
+        <v>6</v>
+      </c>
       <c r="K75" s="173"/>
-      <c r="L75" s="174"/>
-      <c r="M75" s="214"/>
-      <c r="N75" s="215"/>
+      <c r="L75" s="174" t="s">
+        <v>393</v>
+      </c>
+      <c r="M75" s="223" t="s">
+        <v>387</v>
+      </c>
+      <c r="N75" s="224"/>
       <c r="O75" s="170"/>
       <c r="P75" s="170"/>
       <c r="Q75" s="170"/>
     </row>
     <row r="76" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="260"/>
-      <c r="B76" s="258"/>
+      <c r="A76" s="208"/>
+      <c r="B76" s="206"/>
       <c r="C76" s="161">
         <v>18</v>
       </c>
-      <c r="D76" s="175"/>
-      <c r="E76" s="176"/>
-      <c r="F76" s="177"/>
+      <c r="D76" s="175" t="s">
+        <v>378</v>
+      </c>
+      <c r="E76" s="176" t="s">
+        <v>376</v>
+      </c>
+      <c r="F76" s="177" t="s">
+        <v>382</v>
+      </c>
       <c r="G76" s="178"/>
-      <c r="H76" s="178"/>
-      <c r="I76" s="179"/>
-      <c r="J76" s="179"/>
+      <c r="H76" s="178" t="s">
+        <v>386</v>
+      </c>
+      <c r="I76" s="173" t="s">
+        <v>7</v>
+      </c>
+      <c r="J76" s="173" t="s">
+        <v>6</v>
+      </c>
       <c r="K76" s="179"/>
-      <c r="L76" s="180"/>
-      <c r="M76" s="181"/>
+      <c r="L76" s="174" t="s">
+        <v>394</v>
+      </c>
+      <c r="M76" s="275" t="s">
+        <v>388</v>
+      </c>
       <c r="N76" s="182"/>
       <c r="O76" s="170"/>
       <c r="P76" s="170"/>
       <c r="Q76" s="170"/>
     </row>
     <row r="77" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="260"/>
-      <c r="B77" s="258"/>
+      <c r="A77" s="208"/>
+      <c r="B77" s="206"/>
       <c r="C77" s="156">
         <v>19</v>
       </c>
@@ -6639,8 +6778,8 @@
       <c r="Q77" s="170"/>
     </row>
     <row r="78" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="260"/>
-      <c r="B78" s="258"/>
+      <c r="A78" s="208"/>
+      <c r="B78" s="206"/>
       <c r="C78" s="161">
         <v>20</v>
       </c>
@@ -6660,8 +6799,8 @@
       <c r="Q78" s="170"/>
     </row>
     <row r="79" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="260"/>
-      <c r="B79" s="258"/>
+      <c r="A79" s="208"/>
+      <c r="B79" s="206"/>
       <c r="C79" s="156">
         <v>21</v>
       </c>
@@ -6681,8 +6820,8 @@
       <c r="Q79" s="170"/>
     </row>
     <row r="80" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="260"/>
-      <c r="B80" s="258"/>
+      <c r="A80" s="208"/>
+      <c r="B80" s="206"/>
       <c r="C80" s="161">
         <v>22</v>
       </c>
@@ -6702,8 +6841,8 @@
       <c r="Q80" s="170"/>
     </row>
     <row r="81" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="260"/>
-      <c r="B81" s="258"/>
+      <c r="A81" s="208"/>
+      <c r="B81" s="206"/>
       <c r="C81" s="156">
         <v>23</v>
       </c>
@@ -6723,8 +6862,8 @@
       <c r="Q81" s="170"/>
     </row>
     <row r="82" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="260"/>
-      <c r="B82" s="258"/>
+      <c r="A82" s="208"/>
+      <c r="B82" s="206"/>
       <c r="C82" s="161">
         <v>24</v>
       </c>
@@ -6744,8 +6883,8 @@
       <c r="Q82" s="170"/>
     </row>
     <row r="83" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="260"/>
-      <c r="B83" s="258"/>
+      <c r="A83" s="208"/>
+      <c r="B83" s="206"/>
       <c r="C83" s="156">
         <v>25</v>
       </c>
@@ -6765,8 +6904,8 @@
       <c r="Q83" s="170"/>
     </row>
     <row r="84" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="260"/>
-      <c r="B84" s="258"/>
+      <c r="A84" s="208"/>
+      <c r="B84" s="206"/>
       <c r="C84" s="161">
         <v>26</v>
       </c>
@@ -6779,15 +6918,15 @@
       <c r="J84" s="173"/>
       <c r="K84" s="173"/>
       <c r="L84" s="183"/>
-      <c r="M84" s="212"/>
-      <c r="N84" s="213"/>
+      <c r="M84" s="263"/>
+      <c r="N84" s="264"/>
       <c r="O84" s="104"/>
       <c r="P84" s="104"/>
       <c r="Q84" s="104"/>
     </row>
     <row r="85" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="260"/>
-      <c r="B85" s="258"/>
+      <c r="A85" s="208"/>
+      <c r="B85" s="206"/>
       <c r="C85" s="156">
         <v>27</v>
       </c>
@@ -6800,12 +6939,12 @@
       <c r="J85" s="173"/>
       <c r="K85" s="173"/>
       <c r="L85" s="183"/>
-      <c r="M85" s="212"/>
-      <c r="N85" s="213"/>
+      <c r="M85" s="263"/>
+      <c r="N85" s="264"/>
     </row>
     <row r="86" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="260"/>
-      <c r="B86" s="258"/>
+      <c r="A86" s="208"/>
+      <c r="B86" s="206"/>
       <c r="C86" s="161">
         <v>28</v>
       </c>
@@ -6822,8 +6961,8 @@
       <c r="N86" s="182"/>
     </row>
     <row r="87" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="260"/>
-      <c r="B87" s="258"/>
+      <c r="A87" s="208"/>
+      <c r="B87" s="206"/>
       <c r="C87" s="156">
         <v>29</v>
       </c>
@@ -6840,8 +6979,8 @@
       <c r="N87" s="182"/>
     </row>
     <row r="88" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="260"/>
-      <c r="B88" s="258"/>
+      <c r="A88" s="208"/>
+      <c r="B88" s="206"/>
       <c r="C88" s="161">
         <v>30</v>
       </c>
@@ -6858,8 +6997,8 @@
       <c r="N88" s="182"/>
     </row>
     <row r="89" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="260"/>
-      <c r="B89" s="258"/>
+      <c r="A89" s="208"/>
+      <c r="B89" s="206"/>
       <c r="C89" s="156">
         <v>31</v>
       </c>
@@ -6876,8 +7015,8 @@
       <c r="N89" s="182"/>
     </row>
     <row r="90" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="260"/>
-      <c r="B90" s="258"/>
+      <c r="A90" s="208"/>
+      <c r="B90" s="206"/>
       <c r="C90" s="161">
         <v>32</v>
       </c>
@@ -6890,15 +7029,15 @@
       <c r="J90" s="188"/>
       <c r="K90" s="188"/>
       <c r="L90" s="189"/>
-      <c r="M90" s="268"/>
-      <c r="N90" s="269"/>
+      <c r="M90" s="221"/>
+      <c r="N90" s="222"/>
     </row>
     <row r="91" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F91" s="191"/>
-      <c r="G91" s="205"/>
-      <c r="H91" s="205"/>
-      <c r="I91" s="205"/>
-      <c r="J91" s="205"/>
+      <c r="G91" s="267"/>
+      <c r="H91" s="267"/>
+      <c r="I91" s="267"/>
+      <c r="J91" s="267"/>
       <c r="M91" s="104"/>
       <c r="N91" s="104"/>
     </row>
@@ -6906,19 +7045,57 @@
       <c r="F92" s="191" t="s">
         <v>308</v>
       </c>
-      <c r="G92" s="206" t="s">
+      <c r="G92" s="268" t="s">
         <v>309</v>
       </c>
-      <c r="H92" s="206"/>
-      <c r="I92" s="207" t="s">
+      <c r="H92" s="268"/>
+      <c r="I92" s="269" t="s">
         <v>310</v>
       </c>
-      <c r="J92" s="207"/>
+      <c r="J92" s="269"/>
       <c r="M92" s="104"/>
       <c r="N92" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="I91:J91"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="I92:J92"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="M66:N66"/>
+    <mergeCell ref="M67:N67"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="A5:A42"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="M2:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
     <mergeCell ref="B59:B90"/>
     <mergeCell ref="A59:A90"/>
     <mergeCell ref="M43:N43"/>
@@ -6935,44 +7112,6 @@
     <mergeCell ref="M71:N71"/>
     <mergeCell ref="M72:N72"/>
     <mergeCell ref="M73:N73"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M2:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="A5:A42"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="M75:N75"/>
-    <mergeCell ref="M66:N66"/>
-    <mergeCell ref="M67:N67"/>
-    <mergeCell ref="G91:H91"/>
-    <mergeCell ref="I91:J91"/>
-    <mergeCell ref="G92:H92"/>
-    <mergeCell ref="I92:J92"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6991,7 +7130,7 @@
   </sheetPr>
   <dimension ref="A1:CU22"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -8791,7 +8930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
Added support for the polarity switches.
</commit_message>
<xml_diff>
--- a/doc/truth_table_safety_plc.xlsx
+++ b/doc/truth_table_safety_plc.xlsx
@@ -1755,16 +1755,16 @@
     <t>When logical 1 powers motor 2</t>
   </si>
   <si>
-    <t>1 when switching  polarity  until (GERSEMI_POLSW_1_POS1 =  1 AND POLSW_DIR_POS1 = 1) OR (GERSEMI_POLSW_1_POS2 =  1 AND POLSW_DIR_POS2 = 1)</t>
-  </si>
-  <si>
-    <t>1 when switching  polarity  until (GERSEMI_POLSW_2_POS1 =  1 AND POLSW_DIR_POS1 = 1) OR (GERSEMI_POLSW_2_POS2 =  1 AND POLSW_DIR_POS2 = 1)</t>
-  </si>
-  <si>
     <t>1 when requested polarity switch towards pos1</t>
   </si>
   <si>
     <t>1 when requested polarity switch towards pos2</t>
+  </si>
+  <si>
+    <t>1 when switching  polarity  until (GERSEMI_POLSW_1_POS1 =  1 AND POLSW_DIR_POS1 = 1) OR (GERSEMI_POLSW_1_POS2 =  1 AND POLSW_DIR_POS2 = 1) AND NOT GERSEMI_PC_1_EXT_OUT</t>
+  </si>
+  <si>
+    <t>1 when switching  polarity  until (GERSEMI_POLSW_2_POS1 =  1 AND POLSW_DIR_POS1 = 1) OR (GERSEMI_POLSW_2_POS2 =  1 AND POLSW_DIR_POS2 = 1)  AND NOT GERSEMI_PC_2_EXT_OUT</t>
   </si>
 </sst>
 </file>
@@ -2735,7 +2735,7 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="276">
+  <cellXfs count="281">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -3363,9 +3363,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -3373,44 +3370,110 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="49" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -3420,42 +3483,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3505,113 +3532,103 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="18" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="42" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="49" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="18" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="42" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4011,11 +4028,11 @@
   </sheetPr>
   <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="25" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="K47" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="25" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="L66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C73" sqref="A73:XFD73"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4058,67 +4075,67 @@
       <c r="N1" s="86"/>
     </row>
     <row r="2" spans="1:22" s="87" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="245" t="s">
+      <c r="A2" s="222" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="248"/>
-      <c r="C2" s="249"/>
-      <c r="D2" s="255" t="s">
+      <c r="B2" s="225"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="216" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="270" t="s">
+      <c r="E2" s="206" t="s">
         <v>246</v>
       </c>
-      <c r="F2" s="255" t="s">
+      <c r="F2" s="216" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="261" t="s">
+      <c r="G2" s="220" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="262"/>
-      <c r="I2" s="259" t="s">
+      <c r="H2" s="221"/>
+      <c r="I2" s="218" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="259"/>
-      <c r="K2" s="255" t="s">
+      <c r="J2" s="218"/>
+      <c r="K2" s="216" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="257" t="s">
+      <c r="L2" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="231" t="s">
+      <c r="M2" s="235" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="232"/>
+      <c r="N2" s="236"/>
       <c r="O2" s="88"/>
       <c r="P2" s="88"/>
       <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:22" s="87" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="246"/>
-      <c r="B3" s="250"/>
-      <c r="C3" s="251"/>
-      <c r="D3" s="256"/>
-      <c r="E3" s="271"/>
-      <c r="F3" s="256"/>
+      <c r="A3" s="223"/>
+      <c r="B3" s="227"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="217"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="217"/>
       <c r="G3" s="193" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="193" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="260"/>
-      <c r="J3" s="260"/>
-      <c r="K3" s="260"/>
-      <c r="L3" s="258"/>
-      <c r="M3" s="233"/>
-      <c r="N3" s="234"/>
+      <c r="I3" s="219"/>
+      <c r="J3" s="219"/>
+      <c r="K3" s="219"/>
+      <c r="L3" s="215"/>
+      <c r="M3" s="237"/>
+      <c r="N3" s="238"/>
       <c r="O3" s="88"/>
       <c r="P3" s="88"/>
       <c r="Q3" s="88"/>
     </row>
     <row r="4" spans="1:22" s="97" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="247"/>
+      <c r="A4" s="224"/>
       <c r="B4" s="89" t="s">
         <v>14</v>
       </c>
@@ -4144,19 +4161,19 @@
       <c r="L4" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="235" t="s">
+      <c r="M4" s="239" t="s">
         <v>84</v>
       </c>
-      <c r="N4" s="236"/>
+      <c r="N4" s="240"/>
       <c r="O4" s="96"/>
       <c r="P4" s="96"/>
       <c r="Q4" s="96"/>
     </row>
     <row r="5" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="216" t="s">
+      <c r="A5" s="232" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="252" t="s">
+      <c r="B5" s="229" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="98">
@@ -4181,17 +4198,17 @@
       <c r="L5" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="243" t="s">
+      <c r="M5" s="247" t="s">
         <v>202</v>
       </c>
-      <c r="N5" s="244"/>
+      <c r="N5" s="248"/>
       <c r="O5" s="104"/>
       <c r="P5" s="104"/>
       <c r="Q5" s="104"/>
     </row>
     <row r="6" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="217"/>
-      <c r="B6" s="253"/>
+      <c r="A6" s="233"/>
+      <c r="B6" s="230"/>
       <c r="C6" s="106">
         <v>2</v>
       </c>
@@ -4214,17 +4231,17 @@
       <c r="L6" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="241" t="s">
+      <c r="M6" s="245" t="s">
         <v>202</v>
       </c>
-      <c r="N6" s="242"/>
+      <c r="N6" s="246"/>
       <c r="O6" s="104"/>
       <c r="P6" s="104"/>
       <c r="Q6" s="104"/>
     </row>
     <row r="7" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="217"/>
-      <c r="B7" s="253"/>
+      <c r="A7" s="233"/>
+      <c r="B7" s="230"/>
       <c r="C7" s="106">
         <v>3</v>
       </c>
@@ -4247,17 +4264,17 @@
       <c r="L7" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="241" t="s">
+      <c r="M7" s="245" t="s">
         <v>294</v>
       </c>
-      <c r="N7" s="242"/>
+      <c r="N7" s="246"/>
       <c r="O7" s="104"/>
       <c r="P7" s="104"/>
       <c r="Q7" s="104"/>
     </row>
     <row r="8" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="217"/>
-      <c r="B8" s="253"/>
+      <c r="A8" s="233"/>
+      <c r="B8" s="230"/>
       <c r="C8" s="106">
         <v>4</v>
       </c>
@@ -4280,17 +4297,17 @@
       <c r="L8" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="241" t="s">
+      <c r="M8" s="245" t="s">
         <v>295</v>
       </c>
-      <c r="N8" s="242"/>
+      <c r="N8" s="246"/>
       <c r="O8" s="104"/>
       <c r="P8" s="104"/>
       <c r="Q8" s="104"/>
     </row>
     <row r="9" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="217"/>
-      <c r="B9" s="253"/>
+      <c r="A9" s="233"/>
+      <c r="B9" s="230"/>
       <c r="C9" s="106">
         <v>5</v>
       </c>
@@ -4313,17 +4330,17 @@
       <c r="L9" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="241" t="s">
+      <c r="M9" s="245" t="s">
         <v>296</v>
       </c>
-      <c r="N9" s="242"/>
+      <c r="N9" s="246"/>
       <c r="O9" s="104"/>
       <c r="P9" s="104"/>
       <c r="Q9" s="104"/>
     </row>
     <row r="10" spans="1:22" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="217"/>
-      <c r="B10" s="254"/>
+      <c r="A10" s="233"/>
+      <c r="B10" s="231"/>
       <c r="C10" s="113">
         <v>6</v>
       </c>
@@ -4346,17 +4363,17 @@
       <c r="L10" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="241" t="s">
+      <c r="M10" s="245" t="s">
         <v>297</v>
       </c>
-      <c r="N10" s="242"/>
+      <c r="N10" s="246"/>
       <c r="O10" s="104"/>
       <c r="P10" s="104"/>
       <c r="Q10" s="104"/>
     </row>
     <row r="11" spans="1:22" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="217"/>
-      <c r="B11" s="213" t="s">
+      <c r="A11" s="233"/>
+      <c r="B11" s="259" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="119">
@@ -4387,17 +4404,17 @@
       <c r="L11" s="124">
         <v>1</v>
       </c>
-      <c r="M11" s="237" t="s">
+      <c r="M11" s="241" t="s">
         <v>85</v>
       </c>
-      <c r="N11" s="238"/>
+      <c r="N11" s="242"/>
       <c r="O11" s="104"/>
       <c r="P11" s="104"/>
       <c r="Q11" s="104"/>
     </row>
     <row r="12" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="217"/>
-      <c r="B12" s="214"/>
+      <c r="A12" s="233"/>
+      <c r="B12" s="260"/>
       <c r="C12" s="125">
         <v>2</v>
       </c>
@@ -4426,15 +4443,15 @@
       <c r="L12" s="130">
         <v>1</v>
       </c>
-      <c r="M12" s="239"/>
-      <c r="N12" s="240"/>
+      <c r="M12" s="243"/>
+      <c r="N12" s="244"/>
       <c r="O12" s="104"/>
       <c r="P12" s="104"/>
       <c r="Q12" s="104"/>
     </row>
     <row r="13" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="217"/>
-      <c r="B13" s="214"/>
+      <c r="A13" s="233"/>
+      <c r="B13" s="260"/>
       <c r="C13" s="131">
         <v>3</v>
       </c>
@@ -4474,8 +4491,8 @@
       <c r="Q13" s="104"/>
     </row>
     <row r="14" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="217"/>
-      <c r="B14" s="214"/>
+      <c r="A14" s="233"/>
+      <c r="B14" s="260"/>
       <c r="C14" s="125">
         <v>4</v>
       </c>
@@ -4520,8 +4537,8 @@
       <c r="V14" s="137"/>
     </row>
     <row r="15" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="217"/>
-      <c r="B15" s="214"/>
+      <c r="A15" s="233"/>
+      <c r="B15" s="260"/>
       <c r="C15" s="131">
         <v>5</v>
       </c>
@@ -4566,8 +4583,8 @@
       <c r="V15" s="137"/>
     </row>
     <row r="16" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="217"/>
-      <c r="B16" s="214"/>
+      <c r="A16" s="233"/>
+      <c r="B16" s="260"/>
       <c r="C16" s="125">
         <v>6</v>
       </c>
@@ -4610,8 +4627,8 @@
       <c r="V16" s="137"/>
     </row>
     <row r="17" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="217"/>
-      <c r="B17" s="214"/>
+      <c r="A17" s="233"/>
+      <c r="B17" s="260"/>
       <c r="C17" s="131">
         <v>7</v>
       </c>
@@ -4656,8 +4673,8 @@
       <c r="V17" s="137"/>
     </row>
     <row r="18" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="217"/>
-      <c r="B18" s="214"/>
+      <c r="A18" s="233"/>
+      <c r="B18" s="260"/>
       <c r="C18" s="125">
         <v>8</v>
       </c>
@@ -4702,8 +4719,8 @@
       <c r="V18" s="137"/>
     </row>
     <row r="19" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="217"/>
-      <c r="B19" s="214"/>
+      <c r="A19" s="233"/>
+      <c r="B19" s="260"/>
       <c r="C19" s="131">
         <v>9</v>
       </c>
@@ -4748,8 +4765,8 @@
       <c r="V19" s="137"/>
     </row>
     <row r="20" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="217"/>
-      <c r="B20" s="214"/>
+      <c r="A20" s="233"/>
+      <c r="B20" s="260"/>
       <c r="C20" s="125">
         <v>10</v>
       </c>
@@ -4789,8 +4806,8 @@
       <c r="Q20" s="104"/>
     </row>
     <row r="21" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="217"/>
-      <c r="B21" s="214"/>
+      <c r="A21" s="233"/>
+      <c r="B21" s="260"/>
       <c r="C21" s="131">
         <v>11</v>
       </c>
@@ -4830,8 +4847,8 @@
       <c r="Q21" s="104"/>
     </row>
     <row r="22" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="217"/>
-      <c r="B22" s="214"/>
+      <c r="A22" s="233"/>
+      <c r="B22" s="260"/>
       <c r="C22" s="125">
         <v>12</v>
       </c>
@@ -4869,8 +4886,8 @@
       <c r="Q22" s="104"/>
     </row>
     <row r="23" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="217"/>
-      <c r="B23" s="214"/>
+      <c r="A23" s="233"/>
+      <c r="B23" s="260"/>
       <c r="C23" s="131">
         <v>13</v>
       </c>
@@ -4910,8 +4927,8 @@
       <c r="Q23" s="104"/>
     </row>
     <row r="24" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="217"/>
-      <c r="B24" s="214"/>
+      <c r="A24" s="233"/>
+      <c r="B24" s="260"/>
       <c r="C24" s="125">
         <v>14</v>
       </c>
@@ -4951,8 +4968,8 @@
       <c r="Q24" s="104"/>
     </row>
     <row r="25" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="217"/>
-      <c r="B25" s="214"/>
+      <c r="A25" s="233"/>
+      <c r="B25" s="260"/>
       <c r="C25" s="131">
         <v>15</v>
       </c>
@@ -4981,17 +4998,17 @@
       <c r="L25" s="130">
         <v>1</v>
       </c>
-      <c r="M25" s="211" t="s">
+      <c r="M25" s="251" t="s">
         <v>359</v>
       </c>
-      <c r="N25" s="212"/>
+      <c r="N25" s="252"/>
       <c r="O25" s="104"/>
       <c r="P25" s="104"/>
       <c r="Q25" s="104"/>
     </row>
     <row r="26" spans="1:22" s="141" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="217"/>
-      <c r="B26" s="214"/>
+      <c r="A26" s="233"/>
+      <c r="B26" s="260"/>
       <c r="C26" s="131">
         <v>16</v>
       </c>
@@ -5020,17 +5037,17 @@
       <c r="L26" s="130">
         <v>1</v>
       </c>
-      <c r="M26" s="211" t="s">
+      <c r="M26" s="251" t="s">
         <v>46</v>
       </c>
-      <c r="N26" s="212"/>
+      <c r="N26" s="252"/>
       <c r="O26" s="140"/>
       <c r="P26" s="140"/>
       <c r="Q26" s="140"/>
     </row>
     <row r="27" spans="1:22" s="143" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="217"/>
-      <c r="B27" s="214"/>
+      <c r="A27" s="233"/>
+      <c r="B27" s="260"/>
       <c r="C27" s="125">
         <v>17</v>
       </c>
@@ -5059,17 +5076,17 @@
       <c r="L27" s="130">
         <v>1</v>
       </c>
-      <c r="M27" s="211" t="s">
+      <c r="M27" s="251" t="s">
         <v>360</v>
       </c>
-      <c r="N27" s="212"/>
+      <c r="N27" s="252"/>
       <c r="O27" s="142"/>
       <c r="P27" s="142"/>
       <c r="Q27" s="142"/>
     </row>
     <row r="28" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="217"/>
-      <c r="B28" s="214"/>
+      <c r="A28" s="233"/>
+      <c r="B28" s="260"/>
       <c r="C28" s="131">
         <v>18</v>
       </c>
@@ -5098,17 +5115,17 @@
       <c r="L28" s="130">
         <v>1</v>
       </c>
-      <c r="M28" s="211" t="s">
+      <c r="M28" s="251" t="s">
         <v>359</v>
       </c>
-      <c r="N28" s="212"/>
+      <c r="N28" s="252"/>
       <c r="O28" s="104"/>
       <c r="P28" s="104"/>
       <c r="Q28" s="104"/>
     </row>
     <row r="29" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="217"/>
-      <c r="B29" s="214"/>
+      <c r="A29" s="233"/>
+      <c r="B29" s="260"/>
       <c r="C29" s="131">
         <v>19</v>
       </c>
@@ -5137,17 +5154,17 @@
       <c r="L29" s="130">
         <v>1</v>
       </c>
-      <c r="M29" s="211" t="s">
+      <c r="M29" s="251" t="s">
         <v>46</v>
       </c>
-      <c r="N29" s="212"/>
+      <c r="N29" s="252"/>
       <c r="O29" s="104"/>
       <c r="P29" s="104"/>
       <c r="Q29" s="104"/>
     </row>
     <row r="30" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="217"/>
-      <c r="B30" s="214"/>
+      <c r="A30" s="233"/>
+      <c r="B30" s="260"/>
       <c r="C30" s="125">
         <v>20</v>
       </c>
@@ -5176,17 +5193,17 @@
       <c r="L30" s="130">
         <v>1</v>
       </c>
-      <c r="M30" s="211" t="s">
+      <c r="M30" s="251" t="s">
         <v>360</v>
       </c>
-      <c r="N30" s="212"/>
+      <c r="N30" s="252"/>
       <c r="O30" s="104"/>
       <c r="P30" s="104"/>
       <c r="Q30" s="104"/>
     </row>
     <row r="31" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="217"/>
-      <c r="B31" s="214"/>
+      <c r="A31" s="233"/>
+      <c r="B31" s="260"/>
       <c r="C31" s="131">
         <v>21</v>
       </c>
@@ -5222,8 +5239,8 @@
       <c r="Q31" s="104"/>
     </row>
     <row r="32" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="217"/>
-      <c r="B32" s="214"/>
+      <c r="A32" s="233"/>
+      <c r="B32" s="260"/>
       <c r="C32" s="131">
         <v>22</v>
       </c>
@@ -5261,8 +5278,8 @@
       <c r="Q32" s="104"/>
     </row>
     <row r="33" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="217"/>
-      <c r="B33" s="214"/>
+      <c r="A33" s="233"/>
+      <c r="B33" s="260"/>
       <c r="C33" s="131">
         <v>23</v>
       </c>
@@ -5300,8 +5317,8 @@
       <c r="Q33" s="104"/>
     </row>
     <row r="34" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="217"/>
-      <c r="B34" s="214"/>
+      <c r="A34" s="233"/>
+      <c r="B34" s="260"/>
       <c r="C34" s="131">
         <v>24</v>
       </c>
@@ -5339,8 +5356,8 @@
       <c r="Q34" s="104"/>
     </row>
     <row r="35" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="217"/>
-      <c r="B35" s="214"/>
+      <c r="A35" s="233"/>
+      <c r="B35" s="260"/>
       <c r="C35" s="131">
         <v>25</v>
       </c>
@@ -5372,8 +5389,8 @@
       <c r="Q35" s="104"/>
     </row>
     <row r="36" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="217"/>
-      <c r="B36" s="214"/>
+      <c r="A36" s="233"/>
+      <c r="B36" s="260"/>
       <c r="C36" s="131">
         <v>26</v>
       </c>
@@ -5405,8 +5422,8 @@
       <c r="Q36" s="104"/>
     </row>
     <row r="37" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="217"/>
-      <c r="B37" s="214"/>
+      <c r="A37" s="233"/>
+      <c r="B37" s="260"/>
       <c r="C37" s="131">
         <v>27</v>
       </c>
@@ -5438,8 +5455,8 @@
       <c r="Q37" s="104"/>
     </row>
     <row r="38" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="217"/>
-      <c r="B38" s="214"/>
+      <c r="A38" s="233"/>
+      <c r="B38" s="260"/>
       <c r="C38" s="131">
         <v>28</v>
       </c>
@@ -5471,8 +5488,8 @@
       <c r="Q38" s="104"/>
     </row>
     <row r="39" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="217"/>
-      <c r="B39" s="214"/>
+      <c r="A39" s="233"/>
+      <c r="B39" s="260"/>
       <c r="C39" s="131">
         <v>29</v>
       </c>
@@ -5504,8 +5521,8 @@
       <c r="Q39" s="104"/>
     </row>
     <row r="40" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="217"/>
-      <c r="B40" s="214"/>
+      <c r="A40" s="233"/>
+      <c r="B40" s="260"/>
       <c r="C40" s="131">
         <v>30</v>
       </c>
@@ -5537,8 +5554,8 @@
       <c r="Q40" s="104"/>
     </row>
     <row r="41" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="217"/>
-      <c r="B41" s="214"/>
+      <c r="A41" s="233"/>
+      <c r="B41" s="260"/>
       <c r="C41" s="131">
         <v>31</v>
       </c>
@@ -5551,15 +5568,15 @@
       <c r="J41" s="129"/>
       <c r="K41" s="129"/>
       <c r="L41" s="146"/>
-      <c r="M41" s="211"/>
-      <c r="N41" s="212"/>
+      <c r="M41" s="251"/>
+      <c r="N41" s="252"/>
       <c r="O41" s="104"/>
       <c r="P41" s="104"/>
       <c r="Q41" s="104"/>
     </row>
     <row r="42" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="218"/>
-      <c r="B42" s="215"/>
+      <c r="A42" s="234"/>
+      <c r="B42" s="261"/>
       <c r="C42" s="147">
         <v>32</v>
       </c>
@@ -5572,15 +5589,15 @@
       <c r="J42" s="150"/>
       <c r="K42" s="150"/>
       <c r="L42" s="151"/>
-      <c r="M42" s="229"/>
-      <c r="N42" s="230"/>
+      <c r="M42" s="249"/>
+      <c r="N42" s="250"/>
       <c r="O42" s="104"/>
       <c r="P42" s="104"/>
       <c r="Q42" s="104"/>
     </row>
     <row r="43" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="216"/>
-      <c r="B43" s="213" t="s">
+      <c r="A43" s="232"/>
+      <c r="B43" s="259" t="s">
         <v>83</v>
       </c>
       <c r="C43" s="119">
@@ -5607,15 +5624,15 @@
       <c r="L43" s="152" t="s">
         <v>177</v>
       </c>
-      <c r="M43" s="209"/>
-      <c r="N43" s="210"/>
+      <c r="M43" s="257"/>
+      <c r="N43" s="258"/>
       <c r="O43" s="104"/>
       <c r="P43" s="104"/>
       <c r="Q43" s="104"/>
     </row>
     <row r="44" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="217"/>
-      <c r="B44" s="214"/>
+      <c r="A44" s="233"/>
+      <c r="B44" s="260"/>
       <c r="C44" s="131">
         <v>2</v>
       </c>
@@ -5647,8 +5664,8 @@
       <c r="Q44" s="104"/>
     </row>
     <row r="45" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="217"/>
-      <c r="B45" s="214"/>
+      <c r="A45" s="233"/>
+      <c r="B45" s="260"/>
       <c r="C45" s="155">
         <v>3</v>
       </c>
@@ -5673,17 +5690,17 @@
       <c r="L45" s="152">
         <v>1</v>
       </c>
-      <c r="M45" s="211" t="s">
+      <c r="M45" s="251" t="s">
         <v>179</v>
       </c>
-      <c r="N45" s="212"/>
+      <c r="N45" s="252"/>
       <c r="O45" s="104"/>
       <c r="P45" s="104"/>
       <c r="Q45" s="104"/>
     </row>
     <row r="46" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="217"/>
-      <c r="B46" s="214"/>
+      <c r="A46" s="233"/>
+      <c r="B46" s="260"/>
       <c r="C46" s="125">
         <v>4</v>
       </c>
@@ -5717,8 +5734,8 @@
       <c r="Q46" s="104"/>
     </row>
     <row r="47" spans="1:17" s="143" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="217"/>
-      <c r="B47" s="214"/>
+      <c r="A47" s="233"/>
+      <c r="B47" s="260"/>
       <c r="C47" s="125">
         <v>5</v>
       </c>
@@ -5752,8 +5769,8 @@
       <c r="Q47" s="142"/>
     </row>
     <row r="48" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="217"/>
-      <c r="B48" s="214"/>
+      <c r="A48" s="233"/>
+      <c r="B48" s="260"/>
       <c r="C48" s="125">
         <v>6</v>
       </c>
@@ -5787,8 +5804,8 @@
       <c r="Q48" s="104"/>
     </row>
     <row r="49" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="217"/>
-      <c r="B49" s="214"/>
+      <c r="A49" s="233"/>
+      <c r="B49" s="260"/>
       <c r="C49" s="125">
         <v>7</v>
       </c>
@@ -5822,8 +5839,8 @@
       <c r="Q49" s="104"/>
     </row>
     <row r="50" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="217"/>
-      <c r="B50" s="214"/>
+      <c r="A50" s="233"/>
+      <c r="B50" s="260"/>
       <c r="C50" s="125">
         <v>8</v>
       </c>
@@ -5855,8 +5872,8 @@
       <c r="Q50" s="104"/>
     </row>
     <row r="51" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="217"/>
-      <c r="B51" s="214"/>
+      <c r="A51" s="233"/>
+      <c r="B51" s="260"/>
       <c r="C51" s="125">
         <v>9</v>
       </c>
@@ -5888,8 +5905,8 @@
       <c r="Q51" s="104"/>
     </row>
     <row r="52" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="217"/>
-      <c r="B52" s="214"/>
+      <c r="A52" s="233"/>
+      <c r="B52" s="260"/>
       <c r="C52" s="125">
         <v>10</v>
       </c>
@@ -5921,8 +5938,8 @@
       <c r="Q52" s="104"/>
     </row>
     <row r="53" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="217"/>
-      <c r="B53" s="214"/>
+      <c r="A53" s="233"/>
+      <c r="B53" s="260"/>
       <c r="C53" s="125">
         <v>11</v>
       </c>
@@ -5954,8 +5971,8 @@
       <c r="Q53" s="104"/>
     </row>
     <row r="54" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="217"/>
-      <c r="B54" s="214"/>
+      <c r="A54" s="233"/>
+      <c r="B54" s="260"/>
       <c r="C54" s="125">
         <v>12</v>
       </c>
@@ -5975,8 +5992,8 @@
       <c r="Q54" s="104"/>
     </row>
     <row r="55" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="217"/>
-      <c r="B55" s="214"/>
+      <c r="A55" s="233"/>
+      <c r="B55" s="260"/>
       <c r="C55" s="125">
         <v>13</v>
       </c>
@@ -5996,8 +6013,8 @@
       <c r="Q55" s="104"/>
     </row>
     <row r="56" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="217"/>
-      <c r="B56" s="214"/>
+      <c r="A56" s="233"/>
+      <c r="B56" s="260"/>
       <c r="C56" s="125">
         <v>14</v>
       </c>
@@ -6017,8 +6034,8 @@
       <c r="Q56" s="104"/>
     </row>
     <row r="57" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="217"/>
-      <c r="B57" s="214"/>
+      <c r="A57" s="233"/>
+      <c r="B57" s="260"/>
       <c r="C57" s="125">
         <v>15</v>
       </c>
@@ -6038,8 +6055,8 @@
       <c r="Q57" s="104"/>
     </row>
     <row r="58" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="218"/>
-      <c r="B58" s="215"/>
+      <c r="A58" s="234"/>
+      <c r="B58" s="261"/>
       <c r="C58" s="125">
         <v>16</v>
       </c>
@@ -6059,10 +6076,10 @@
       <c r="Q58" s="104"/>
     </row>
     <row r="59" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="207" t="s">
+      <c r="A59" s="255" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="205" t="s">
+      <c r="B59" s="253" t="s">
         <v>55</v>
       </c>
       <c r="C59" s="156">
@@ -6087,21 +6104,21 @@
       <c r="J59" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="K59" s="199" t="s">
+      <c r="K59" s="278" t="s">
         <v>2</v>
       </c>
-      <c r="L59" s="200" t="s">
+      <c r="L59" s="279" t="s">
         <v>236</v>
       </c>
-      <c r="M59" s="219"/>
-      <c r="N59" s="220"/>
+      <c r="M59" s="262"/>
+      <c r="N59" s="263"/>
       <c r="O59" s="104"/>
       <c r="P59" s="104"/>
       <c r="Q59" s="104"/>
     </row>
     <row r="60" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="208"/>
-      <c r="B60" s="206"/>
+      <c r="A60" s="256"/>
+      <c r="B60" s="254"/>
       <c r="C60" s="161">
         <v>2</v>
       </c>
@@ -6122,10 +6139,10 @@
       <c r="J60" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K60" s="110" t="s">
+      <c r="K60" s="273" t="s">
         <v>86</v>
       </c>
-      <c r="L60" s="111" t="s">
+      <c r="L60" s="274" t="s">
         <v>183</v>
       </c>
       <c r="M60" s="166" t="s">
@@ -6139,8 +6156,8 @@
       <c r="Q60" s="104"/>
     </row>
     <row r="61" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="208"/>
-      <c r="B61" s="206"/>
+      <c r="A61" s="256"/>
+      <c r="B61" s="254"/>
       <c r="C61" s="156">
         <v>3</v>
       </c>
@@ -6154,19 +6171,19 @@
         <v>143</v>
       </c>
       <c r="G61" s="165"/>
-      <c r="H61" s="201" t="s">
+      <c r="H61" s="200" t="s">
         <v>241</v>
       </c>
-      <c r="I61" s="202" t="s">
+      <c r="I61" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="J61" s="202" t="s">
+      <c r="J61" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="K61" s="202" t="s">
+      <c r="K61" s="273" t="s">
         <v>86</v>
       </c>
-      <c r="L61" s="203" t="s">
+      <c r="L61" s="274" t="s">
         <v>182</v>
       </c>
       <c r="M61" s="166" t="s">
@@ -6180,8 +6197,8 @@
       <c r="Q61" s="104"/>
     </row>
     <row r="62" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="208"/>
-      <c r="B62" s="206"/>
+      <c r="A62" s="256"/>
+      <c r="B62" s="254"/>
       <c r="C62" s="161">
         <v>4</v>
       </c>
@@ -6195,19 +6212,19 @@
         <v>144</v>
       </c>
       <c r="G62" s="165"/>
-      <c r="H62" s="201" t="s">
+      <c r="H62" s="200" t="s">
         <v>242</v>
       </c>
-      <c r="I62" s="202" t="s">
+      <c r="I62" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="J62" s="202" t="s">
+      <c r="J62" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="K62" s="202" t="s">
+      <c r="K62" s="273" t="s">
         <v>86</v>
       </c>
-      <c r="L62" s="203" t="s">
+      <c r="L62" s="274" t="s">
         <v>182</v>
       </c>
       <c r="M62" s="168" t="s">
@@ -6221,8 +6238,8 @@
       <c r="Q62" s="104"/>
     </row>
     <row r="63" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="208"/>
-      <c r="B63" s="206"/>
+      <c r="A63" s="256"/>
+      <c r="B63" s="254"/>
       <c r="C63" s="156">
         <v>5</v>
       </c>
@@ -6243,10 +6260,10 @@
       <c r="J63" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K63" s="110" t="s">
+      <c r="K63" s="273" t="s">
         <v>86</v>
       </c>
-      <c r="L63" s="111" t="s">
+      <c r="L63" s="274" t="s">
         <v>183</v>
       </c>
       <c r="M63" s="166" t="s">
@@ -6260,8 +6277,8 @@
       <c r="Q63" s="170"/>
     </row>
     <row r="64" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="208"/>
-      <c r="B64" s="206"/>
+      <c r="A64" s="256"/>
+      <c r="B64" s="254"/>
       <c r="C64" s="161">
         <v>6</v>
       </c>
@@ -6275,19 +6292,19 @@
         <v>143</v>
       </c>
       <c r="G64" s="165"/>
-      <c r="H64" s="201" t="s">
+      <c r="H64" s="200" t="s">
         <v>243</v>
       </c>
-      <c r="I64" s="202" t="s">
+      <c r="I64" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="J64" s="202" t="s">
+      <c r="J64" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="K64" s="202" t="s">
+      <c r="K64" s="273" t="s">
         <v>86</v>
       </c>
-      <c r="L64" s="203" t="s">
+      <c r="L64" s="274" t="s">
         <v>182</v>
       </c>
       <c r="M64" s="166" t="s">
@@ -6301,8 +6318,8 @@
       <c r="Q64" s="170"/>
     </row>
     <row r="65" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="208"/>
-      <c r="B65" s="206"/>
+      <c r="A65" s="256"/>
+      <c r="B65" s="254"/>
       <c r="C65" s="156">
         <v>7</v>
       </c>
@@ -6316,19 +6333,19 @@
         <v>144</v>
       </c>
       <c r="G65" s="165"/>
-      <c r="H65" s="201" t="s">
+      <c r="H65" s="200" t="s">
         <v>244</v>
       </c>
-      <c r="I65" s="202" t="s">
+      <c r="I65" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="J65" s="202" t="s">
+      <c r="J65" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="K65" s="202" t="s">
+      <c r="K65" s="273" t="s">
         <v>86</v>
       </c>
-      <c r="L65" s="203" t="s">
+      <c r="L65" s="274" t="s">
         <v>182</v>
       </c>
       <c r="M65" s="168" t="s">
@@ -6342,8 +6359,8 @@
       <c r="Q65" s="170"/>
     </row>
     <row r="66" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="208"/>
-      <c r="B66" s="206"/>
+      <c r="A66" s="256"/>
+      <c r="B66" s="254"/>
       <c r="C66" s="161">
         <v>8</v>
       </c>
@@ -6357,32 +6374,32 @@
         <v>27</v>
       </c>
       <c r="G66" s="165"/>
-      <c r="H66" s="202" t="s">
+      <c r="H66" s="201" t="s">
         <v>237</v>
       </c>
-      <c r="I66" s="202" t="s">
+      <c r="I66" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="J66" s="202" t="s">
+      <c r="J66" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="K66" s="202" t="s">
+      <c r="K66" s="273" t="s">
         <v>2</v>
       </c>
-      <c r="L66" s="204" t="s">
+      <c r="L66" s="280" t="s">
         <v>181</v>
       </c>
-      <c r="M66" s="265" t="s">
+      <c r="M66" s="212" t="s">
         <v>47</v>
       </c>
-      <c r="N66" s="266"/>
+      <c r="N66" s="213"/>
       <c r="O66" s="170"/>
       <c r="P66" s="170"/>
       <c r="Q66" s="170"/>
     </row>
     <row r="67" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="208"/>
-      <c r="B67" s="206"/>
+      <c r="A67" s="256"/>
+      <c r="B67" s="254"/>
       <c r="C67" s="156">
         <v>9</v>
       </c>
@@ -6396,32 +6413,32 @@
         <v>27</v>
       </c>
       <c r="G67" s="165"/>
-      <c r="H67" s="202" t="s">
+      <c r="H67" s="201" t="s">
         <v>238</v>
       </c>
-      <c r="I67" s="202" t="s">
+      <c r="I67" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="J67" s="202" t="s">
+      <c r="J67" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="K67" s="202" t="s">
+      <c r="K67" s="273" t="s">
         <v>2</v>
       </c>
-      <c r="L67" s="204" t="s">
+      <c r="L67" s="280" t="s">
         <v>181</v>
       </c>
-      <c r="M67" s="265" t="s">
+      <c r="M67" s="212" t="s">
         <v>47</v>
       </c>
-      <c r="N67" s="266"/>
+      <c r="N67" s="213"/>
       <c r="O67" s="170"/>
       <c r="P67" s="170"/>
       <c r="Q67" s="170"/>
     </row>
     <row r="68" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="208"/>
-      <c r="B68" s="206"/>
+      <c r="A68" s="256"/>
+      <c r="B68" s="254"/>
       <c r="C68" s="161">
         <v>10</v>
       </c>
@@ -6435,32 +6452,32 @@
         <v>176</v>
       </c>
       <c r="G68" s="165"/>
-      <c r="H68" s="202" t="s">
+      <c r="H68" s="201" t="s">
         <v>239</v>
       </c>
-      <c r="I68" s="202" t="s">
+      <c r="I68" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="J68" s="202" t="s">
+      <c r="J68" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="K68" s="202" t="s">
+      <c r="K68" s="273" t="s">
         <v>2</v>
       </c>
-      <c r="L68" s="203" t="s">
+      <c r="L68" s="274" t="s">
         <v>180</v>
       </c>
-      <c r="M68" s="223" t="s">
+      <c r="M68" s="208" t="s">
         <v>367</v>
       </c>
-      <c r="N68" s="224"/>
+      <c r="N68" s="209"/>
       <c r="O68" s="170"/>
       <c r="P68" s="170"/>
       <c r="Q68" s="170"/>
     </row>
     <row r="69" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="208"/>
-      <c r="B69" s="206"/>
+      <c r="A69" s="256"/>
+      <c r="B69" s="254"/>
       <c r="C69" s="156">
         <v>11</v>
       </c>
@@ -6474,32 +6491,32 @@
         <v>176</v>
       </c>
       <c r="G69" s="165"/>
-      <c r="H69" s="202" t="s">
+      <c r="H69" s="201" t="s">
         <v>240</v>
       </c>
-      <c r="I69" s="202" t="s">
+      <c r="I69" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="J69" s="202" t="s">
+      <c r="J69" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="K69" s="202" t="s">
+      <c r="K69" s="273" t="s">
         <v>2</v>
       </c>
-      <c r="L69" s="203" t="s">
+      <c r="L69" s="274" t="s">
         <v>180</v>
       </c>
-      <c r="M69" s="223" t="s">
+      <c r="M69" s="208" t="s">
         <v>367</v>
       </c>
-      <c r="N69" s="224"/>
+      <c r="N69" s="209"/>
       <c r="O69" s="170"/>
       <c r="P69" s="170"/>
       <c r="Q69" s="170"/>
     </row>
     <row r="70" spans="1:17" s="171" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="208"/>
-      <c r="B70" s="206"/>
+      <c r="A70" s="256"/>
+      <c r="B70" s="254"/>
       <c r="C70" s="161">
         <v>12</v>
       </c>
@@ -6513,30 +6530,30 @@
         <v>145</v>
       </c>
       <c r="G70" s="165"/>
-      <c r="H70" s="201" t="s">
+      <c r="H70" s="200" t="s">
         <v>232</v>
       </c>
-      <c r="I70" s="202" t="s">
+      <c r="I70" s="201" t="s">
         <v>7</v>
       </c>
-      <c r="J70" s="202" t="s">
+      <c r="J70" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="K70" s="202" t="s">
+      <c r="K70" s="273" t="s">
         <v>322</v>
       </c>
-      <c r="L70" s="203" t="s">
+      <c r="L70" s="274" t="s">
         <v>304</v>
       </c>
-      <c r="M70" s="225"/>
-      <c r="N70" s="226"/>
+      <c r="M70" s="266"/>
+      <c r="N70" s="267"/>
       <c r="O70" s="170"/>
       <c r="P70" s="170"/>
       <c r="Q70" s="170"/>
     </row>
     <row r="71" spans="1:17" s="171" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="208"/>
-      <c r="B71" s="206"/>
+      <c r="A71" s="256"/>
+      <c r="B71" s="254"/>
       <c r="C71" s="156">
         <v>13</v>
       </c>
@@ -6550,30 +6567,30 @@
         <v>146</v>
       </c>
       <c r="G71" s="165"/>
-      <c r="H71" s="201" t="s">
+      <c r="H71" s="275" t="s">
         <v>233</v>
       </c>
-      <c r="I71" s="202" t="s">
+      <c r="I71" s="273" t="s">
         <v>7</v>
       </c>
-      <c r="J71" s="202" t="s">
+      <c r="J71" s="273" t="s">
         <v>6</v>
       </c>
-      <c r="K71" s="202" t="s">
+      <c r="K71" s="273" t="s">
         <v>322</v>
       </c>
-      <c r="L71" s="203" t="s">
+      <c r="L71" s="274" t="s">
         <v>304</v>
       </c>
-      <c r="M71" s="225"/>
-      <c r="N71" s="226"/>
+      <c r="M71" s="266"/>
+      <c r="N71" s="267"/>
       <c r="O71" s="170"/>
       <c r="P71" s="170"/>
       <c r="Q71" s="170"/>
     </row>
     <row r="72" spans="1:17" s="171" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="208"/>
-      <c r="B72" s="206"/>
+      <c r="A72" s="256"/>
+      <c r="B72" s="254"/>
       <c r="C72" s="161">
         <v>14</v>
       </c>
@@ -6587,30 +6604,30 @@
         <v>147</v>
       </c>
       <c r="G72" s="165"/>
-      <c r="H72" s="201" t="s">
+      <c r="H72" s="275" t="s">
         <v>234</v>
       </c>
-      <c r="I72" s="202" t="s">
+      <c r="I72" s="273" t="s">
         <v>7</v>
       </c>
-      <c r="J72" s="202" t="s">
+      <c r="J72" s="273" t="s">
         <v>6</v>
       </c>
-      <c r="K72" s="202" t="s">
+      <c r="K72" s="273" t="s">
         <v>322</v>
       </c>
-      <c r="L72" s="203" t="s">
+      <c r="L72" s="274" t="s">
         <v>304</v>
       </c>
-      <c r="M72" s="227"/>
-      <c r="N72" s="228"/>
+      <c r="M72" s="268"/>
+      <c r="N72" s="269"/>
       <c r="O72" s="170"/>
       <c r="P72" s="170"/>
       <c r="Q72" s="170"/>
     </row>
     <row r="73" spans="1:17" s="171" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="208"/>
-      <c r="B73" s="206"/>
+      <c r="A73" s="256"/>
+      <c r="B73" s="254"/>
       <c r="C73" s="156">
         <v>15</v>
       </c>
@@ -6624,30 +6641,30 @@
         <v>379</v>
       </c>
       <c r="G73" s="165"/>
-      <c r="H73" s="173" t="s">
+      <c r="H73" s="273" t="s">
         <v>383</v>
       </c>
-      <c r="I73" s="173" t="s">
+      <c r="I73" s="273" t="s">
         <v>7</v>
       </c>
-      <c r="J73" s="173" t="s">
+      <c r="J73" s="273" t="s">
         <v>6</v>
       </c>
-      <c r="K73" s="173"/>
-      <c r="L73" s="174" t="s">
-        <v>391</v>
-      </c>
-      <c r="M73" s="223" t="s">
+      <c r="K73" s="273"/>
+      <c r="L73" s="274" t="s">
+        <v>393</v>
+      </c>
+      <c r="M73" s="208" t="s">
         <v>389</v>
       </c>
-      <c r="N73" s="224"/>
+      <c r="N73" s="209"/>
       <c r="O73" s="170"/>
       <c r="P73" s="170"/>
       <c r="Q73" s="170"/>
     </row>
     <row r="74" spans="1:17" s="171" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="208"/>
-      <c r="B74" s="206"/>
+      <c r="A74" s="256"/>
+      <c r="B74" s="254"/>
       <c r="C74" s="161">
         <v>16</v>
       </c>
@@ -6661,30 +6678,30 @@
         <v>380</v>
       </c>
       <c r="G74" s="165"/>
-      <c r="H74" s="165" t="s">
+      <c r="H74" s="275" t="s">
         <v>384</v>
       </c>
-      <c r="I74" s="173" t="s">
+      <c r="I74" s="273" t="s">
         <v>7</v>
       </c>
-      <c r="J74" s="173" t="s">
+      <c r="J74" s="273" t="s">
         <v>6</v>
       </c>
-      <c r="K74" s="173"/>
-      <c r="L74" s="174" t="s">
-        <v>392</v>
-      </c>
-      <c r="M74" s="223" t="s">
+      <c r="K74" s="273"/>
+      <c r="L74" s="274" t="s">
+        <v>394</v>
+      </c>
+      <c r="M74" s="208" t="s">
         <v>390</v>
       </c>
-      <c r="N74" s="224"/>
+      <c r="N74" s="209"/>
       <c r="O74" s="170"/>
       <c r="P74" s="170"/>
       <c r="Q74" s="170"/>
     </row>
     <row r="75" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="208"/>
-      <c r="B75" s="206"/>
+      <c r="A75" s="256"/>
+      <c r="B75" s="254"/>
       <c r="C75" s="156">
         <v>17</v>
       </c>
@@ -6698,30 +6715,30 @@
         <v>381</v>
       </c>
       <c r="G75" s="165"/>
-      <c r="H75" s="165" t="s">
+      <c r="H75" s="275" t="s">
         <v>385</v>
       </c>
-      <c r="I75" s="173" t="s">
+      <c r="I75" s="273" t="s">
         <v>7</v>
       </c>
-      <c r="J75" s="173" t="s">
+      <c r="J75" s="273" t="s">
         <v>6</v>
       </c>
-      <c r="K75" s="173"/>
-      <c r="L75" s="174" t="s">
-        <v>393</v>
-      </c>
-      <c r="M75" s="223" t="s">
+      <c r="K75" s="273"/>
+      <c r="L75" s="274" t="s">
+        <v>391</v>
+      </c>
+      <c r="M75" s="208" t="s">
         <v>387</v>
       </c>
-      <c r="N75" s="224"/>
+      <c r="N75" s="209"/>
       <c r="O75" s="170"/>
       <c r="P75" s="170"/>
       <c r="Q75" s="170"/>
     </row>
     <row r="76" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="208"/>
-      <c r="B76" s="206"/>
+      <c r="A76" s="256"/>
+      <c r="B76" s="254"/>
       <c r="C76" s="161">
         <v>18</v>
       </c>
@@ -6735,20 +6752,20 @@
         <v>382</v>
       </c>
       <c r="G76" s="178"/>
-      <c r="H76" s="178" t="s">
+      <c r="H76" s="276" t="s">
         <v>386</v>
       </c>
-      <c r="I76" s="173" t="s">
+      <c r="I76" s="273" t="s">
         <v>7</v>
       </c>
-      <c r="J76" s="173" t="s">
+      <c r="J76" s="273" t="s">
         <v>6</v>
       </c>
-      <c r="K76" s="179"/>
-      <c r="L76" s="174" t="s">
-        <v>394</v>
-      </c>
-      <c r="M76" s="275" t="s">
+      <c r="K76" s="277"/>
+      <c r="L76" s="274" t="s">
+        <v>392</v>
+      </c>
+      <c r="M76" s="202" t="s">
         <v>388</v>
       </c>
       <c r="N76" s="182"/>
@@ -6757,8 +6774,8 @@
       <c r="Q76" s="170"/>
     </row>
     <row r="77" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="208"/>
-      <c r="B77" s="206"/>
+      <c r="A77" s="256"/>
+      <c r="B77" s="254"/>
       <c r="C77" s="156">
         <v>19</v>
       </c>
@@ -6778,8 +6795,8 @@
       <c r="Q77" s="170"/>
     </row>
     <row r="78" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="208"/>
-      <c r="B78" s="206"/>
+      <c r="A78" s="256"/>
+      <c r="B78" s="254"/>
       <c r="C78" s="161">
         <v>20</v>
       </c>
@@ -6799,8 +6816,8 @@
       <c r="Q78" s="170"/>
     </row>
     <row r="79" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="208"/>
-      <c r="B79" s="206"/>
+      <c r="A79" s="256"/>
+      <c r="B79" s="254"/>
       <c r="C79" s="156">
         <v>21</v>
       </c>
@@ -6820,8 +6837,8 @@
       <c r="Q79" s="170"/>
     </row>
     <row r="80" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="208"/>
-      <c r="B80" s="206"/>
+      <c r="A80" s="256"/>
+      <c r="B80" s="254"/>
       <c r="C80" s="161">
         <v>22</v>
       </c>
@@ -6841,8 +6858,8 @@
       <c r="Q80" s="170"/>
     </row>
     <row r="81" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="208"/>
-      <c r="B81" s="206"/>
+      <c r="A81" s="256"/>
+      <c r="B81" s="254"/>
       <c r="C81" s="156">
         <v>23</v>
       </c>
@@ -6862,8 +6879,8 @@
       <c r="Q81" s="170"/>
     </row>
     <row r="82" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="208"/>
-      <c r="B82" s="206"/>
+      <c r="A82" s="256"/>
+      <c r="B82" s="254"/>
       <c r="C82" s="161">
         <v>24</v>
       </c>
@@ -6883,8 +6900,8 @@
       <c r="Q82" s="170"/>
     </row>
     <row r="83" spans="1:17" s="171" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="208"/>
-      <c r="B83" s="206"/>
+      <c r="A83" s="256"/>
+      <c r="B83" s="254"/>
       <c r="C83" s="156">
         <v>25</v>
       </c>
@@ -6904,8 +6921,8 @@
       <c r="Q83" s="170"/>
     </row>
     <row r="84" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="208"/>
-      <c r="B84" s="206"/>
+      <c r="A84" s="256"/>
+      <c r="B84" s="254"/>
       <c r="C84" s="161">
         <v>26</v>
       </c>
@@ -6918,15 +6935,15 @@
       <c r="J84" s="173"/>
       <c r="K84" s="173"/>
       <c r="L84" s="183"/>
-      <c r="M84" s="263"/>
-      <c r="N84" s="264"/>
+      <c r="M84" s="210"/>
+      <c r="N84" s="211"/>
       <c r="O84" s="104"/>
       <c r="P84" s="104"/>
       <c r="Q84" s="104"/>
     </row>
     <row r="85" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="208"/>
-      <c r="B85" s="206"/>
+      <c r="A85" s="256"/>
+      <c r="B85" s="254"/>
       <c r="C85" s="156">
         <v>27</v>
       </c>
@@ -6939,12 +6956,12 @@
       <c r="J85" s="173"/>
       <c r="K85" s="173"/>
       <c r="L85" s="183"/>
-      <c r="M85" s="263"/>
-      <c r="N85" s="264"/>
+      <c r="M85" s="210"/>
+      <c r="N85" s="211"/>
     </row>
     <row r="86" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="208"/>
-      <c r="B86" s="206"/>
+      <c r="A86" s="256"/>
+      <c r="B86" s="254"/>
       <c r="C86" s="161">
         <v>28</v>
       </c>
@@ -6961,8 +6978,8 @@
       <c r="N86" s="182"/>
     </row>
     <row r="87" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="208"/>
-      <c r="B87" s="206"/>
+      <c r="A87" s="256"/>
+      <c r="B87" s="254"/>
       <c r="C87" s="156">
         <v>29</v>
       </c>
@@ -6979,8 +6996,8 @@
       <c r="N87" s="182"/>
     </row>
     <row r="88" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="208"/>
-      <c r="B88" s="206"/>
+      <c r="A88" s="256"/>
+      <c r="B88" s="254"/>
       <c r="C88" s="161">
         <v>30</v>
       </c>
@@ -6997,8 +7014,8 @@
       <c r="N88" s="182"/>
     </row>
     <row r="89" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="208"/>
-      <c r="B89" s="206"/>
+      <c r="A89" s="256"/>
+      <c r="B89" s="254"/>
       <c r="C89" s="156">
         <v>31</v>
       </c>
@@ -7015,8 +7032,8 @@
       <c r="N89" s="182"/>
     </row>
     <row r="90" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="208"/>
-      <c r="B90" s="206"/>
+      <c r="A90" s="256"/>
+      <c r="B90" s="254"/>
       <c r="C90" s="161">
         <v>32</v>
       </c>
@@ -7029,15 +7046,15 @@
       <c r="J90" s="188"/>
       <c r="K90" s="188"/>
       <c r="L90" s="189"/>
-      <c r="M90" s="221"/>
-      <c r="N90" s="222"/>
+      <c r="M90" s="264"/>
+      <c r="N90" s="265"/>
     </row>
     <row r="91" spans="1:17" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F91" s="191"/>
-      <c r="G91" s="267"/>
-      <c r="H91" s="267"/>
-      <c r="I91" s="267"/>
-      <c r="J91" s="267"/>
+      <c r="G91" s="203"/>
+      <c r="H91" s="203"/>
+      <c r="I91" s="203"/>
+      <c r="J91" s="203"/>
       <c r="M91" s="104"/>
       <c r="N91" s="104"/>
     </row>
@@ -7045,57 +7062,19 @@
       <c r="F92" s="191" t="s">
         <v>308</v>
       </c>
-      <c r="G92" s="268" t="s">
+      <c r="G92" s="204" t="s">
         <v>309</v>
       </c>
-      <c r="H92" s="268"/>
-      <c r="I92" s="269" t="s">
+      <c r="H92" s="204"/>
+      <c r="I92" s="205" t="s">
         <v>310</v>
       </c>
-      <c r="J92" s="269"/>
+      <c r="J92" s="205"/>
       <c r="M92" s="104"/>
       <c r="N92" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="G91:H91"/>
-    <mergeCell ref="I91:J91"/>
-    <mergeCell ref="G92:H92"/>
-    <mergeCell ref="I92:J92"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="M75:N75"/>
-    <mergeCell ref="M66:N66"/>
-    <mergeCell ref="M67:N67"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="A5:A42"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="M2:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
     <mergeCell ref="B59:B90"/>
     <mergeCell ref="A59:A90"/>
     <mergeCell ref="M43:N43"/>
@@ -7112,6 +7091,44 @@
     <mergeCell ref="M71:N71"/>
     <mergeCell ref="M72:N72"/>
     <mergeCell ref="M73:N73"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M2:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="A5:A42"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="M66:N66"/>
+    <mergeCell ref="M67:N67"/>
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="I91:J91"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="I92:J92"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8643,7 +8660,7 @@
       <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="272" t="s">
+      <c r="A2" s="270" t="s">
         <v>155</v>
       </c>
       <c r="B2" s="50">
@@ -8679,7 +8696,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="273"/>
+      <c r="A3" s="271"/>
       <c r="B3" s="37">
         <v>2</v>
       </c>
@@ -8703,7 +8720,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="273"/>
+      <c r="A4" s="271"/>
       <c r="B4" s="79">
         <v>3</v>
       </c>
@@ -8737,7 +8754,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="273"/>
+      <c r="A5" s="271"/>
       <c r="B5" s="50">
         <v>4</v>
       </c>
@@ -8771,7 +8788,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="273"/>
+      <c r="A6" s="271"/>
       <c r="B6" s="37">
         <v>5</v>
       </c>
@@ -8795,7 +8812,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="274"/>
+      <c r="A7" s="272"/>
       <c r="B7" s="50">
         <v>6</v>
       </c>
@@ -8843,7 +8860,7 @@
       <c r="L8" s="56"/>
     </row>
     <row r="9" spans="1:12" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="272" t="s">
+      <c r="A9" s="270" t="s">
         <v>156</v>
       </c>
       <c r="B9" s="50">
@@ -8879,7 +8896,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="274"/>
+      <c r="A10" s="272"/>
       <c r="B10" s="50">
         <v>2</v>
       </c>

</xml_diff>